<commit_message>
Improved documentation; fixed bug.
</commit_message>
<xml_diff>
--- a/dictionaries/TOMES_Entity_Dictionary.xlsx
+++ b/dictionaries/TOMES_Entity_Dictionary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin\Dropbox\TOMES\GitHub\tomes_tool\NLP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin\Dropbox\TOMES\GitHub\tomes_entities\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2700" windowWidth="20400" windowHeight="10410"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="20400" windowHeight="10410"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -1719,9 +1719,6 @@
     <t>[0]{4}[0-9]{8}</t>
   </si>
   <si>
-    <t>Patterns using regular expressions are highlighted in green via Conditional Formatting. You can also search the "patter" column for a "[" character to find regular expressions.</t>
-  </si>
-  <si>
     <t>[0-9]{2}-[0-9]{7}([a-zA-Z]|[0-9]{3}){0,1}</t>
   </si>
   <si>
@@ -2740,6 +2737,9 @@
   </si>
   <si>
     <t>For information on the "Entities" worksheet schema, please see "entity_dictionary_template.xlsx".</t>
+  </si>
+  <si>
+    <t>Patterns using regular expressions and TOMES Patterns are highlighted in green via Conditional Formatting.</t>
   </si>
 </sst>
 </file>
@@ -3191,18 +3191,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>563</v>
+        <v>903</v>
       </c>
     </row>
   </sheetData>
@@ -3251,7 +3253,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>5</v>
@@ -3271,7 +3273,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>14</v>
@@ -3291,7 +3293,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>6</v>
@@ -3311,7 +3313,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>7</v>
@@ -3331,7 +3333,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>8</v>
@@ -3351,7 +3353,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B7" s="28" t="s">
         <v>9</v>
@@ -3371,7 +3373,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>10</v>
@@ -3391,7 +3393,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>11</v>
@@ -3411,7 +3413,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>16</v>
@@ -3431,7 +3433,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>15</v>
@@ -3451,7 +3453,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>26</v>
@@ -3471,7 +3473,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>29</v>
@@ -3491,7 +3493,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>30</v>
@@ -3511,7 +3513,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>31</v>
@@ -3531,7 +3533,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>32</v>
@@ -3551,7 +3553,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>33</v>
@@ -3571,7 +3573,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>34</v>
@@ -3591,7 +3593,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>35</v>
@@ -3611,7 +3613,7 @@
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B20" s="28" t="s">
         <v>36</v>
@@ -3631,7 +3633,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>38</v>
@@ -3651,7 +3653,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>40</v>
@@ -3671,7 +3673,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>42</v>
@@ -3691,7 +3693,7 @@
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>44</v>
@@ -3711,7 +3713,7 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>46</v>
@@ -3731,7 +3733,7 @@
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>48</v>
@@ -3751,7 +3753,7 @@
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>50</v>
@@ -3771,7 +3773,7 @@
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>52</v>
@@ -3791,7 +3793,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>53</v>
@@ -3811,7 +3813,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>55</v>
@@ -3831,7 +3833,7 @@
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>56</v>
@@ -3851,7 +3853,7 @@
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>58</v>
@@ -3871,7 +3873,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>60</v>
@@ -3891,7 +3893,7 @@
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B34" s="28" t="s">
         <v>62</v>
@@ -3911,7 +3913,7 @@
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>64</v>
@@ -3931,7 +3933,7 @@
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B36" s="28" t="s">
         <v>66</v>
@@ -3951,7 +3953,7 @@
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>68</v>
@@ -3971,7 +3973,7 @@
     </row>
     <row r="38" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>78</v>
@@ -3991,7 +3993,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B39" s="28" t="s">
         <v>80</v>
@@ -4011,7 +4013,7 @@
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>81</v>
@@ -4031,7 +4033,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B41" s="28" t="s">
         <v>82</v>
@@ -4051,7 +4053,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B42" s="28" t="s">
         <v>83</v>
@@ -4071,7 +4073,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B43" s="28" t="s">
         <v>84</v>
@@ -4091,7 +4093,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B44" s="28" t="s">
         <v>85</v>
@@ -4111,7 +4113,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B45" s="28" t="s">
         <v>86</v>
@@ -4131,7 +4133,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B46" s="28" t="s">
         <v>87</v>
@@ -4151,7 +4153,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B47" s="28" t="s">
         <v>88</v>
@@ -4171,7 +4173,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B48" s="28" t="s">
         <v>89</v>
@@ -4191,7 +4193,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B49" s="28" t="s">
         <v>90</v>
@@ -4211,7 +4213,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B50" s="28" t="s">
         <v>91</v>
@@ -4231,7 +4233,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B51" s="28" t="s">
         <v>92</v>
@@ -4251,7 +4253,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B52" s="28" t="s">
         <v>93</v>
@@ -4271,7 +4273,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B53" s="28" t="s">
         <v>94</v>
@@ -4291,7 +4293,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B54" s="28" t="s">
         <v>95</v>
@@ -4311,7 +4313,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B55" s="29" t="s">
         <v>115</v>
@@ -4331,7 +4333,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B56" s="28" t="s">
         <v>117</v>
@@ -4351,7 +4353,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B57" s="28" t="s">
         <v>119</v>
@@ -4371,7 +4373,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B58" s="28" t="s">
         <v>120</v>
@@ -4391,7 +4393,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B59" s="28" t="s">
         <v>122</v>
@@ -4411,7 +4413,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B60" s="28" t="s">
         <v>124</v>
@@ -4431,7 +4433,7 @@
     </row>
     <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B61" s="28" t="s">
         <v>126</v>
@@ -4451,7 +4453,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B62" s="28" t="s">
         <v>128</v>
@@ -4471,7 +4473,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B63" s="28" t="s">
         <v>349</v>
@@ -4491,7 +4493,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B64" s="28" t="s">
         <v>131</v>
@@ -4511,7 +4513,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B65" s="28" t="s">
         <v>133</v>
@@ -4531,7 +4533,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B66" s="28" t="s">
         <v>134</v>
@@ -4551,7 +4553,7 @@
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B67" s="28" t="s">
         <v>135</v>
@@ -4571,7 +4573,7 @@
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B68" s="28" t="s">
         <v>136</v>
@@ -4591,7 +4593,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B69" s="28" t="s">
         <v>137</v>
@@ -4611,7 +4613,7 @@
     </row>
     <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B70" s="28" t="s">
         <v>139</v>
@@ -4631,7 +4633,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B71" s="28" t="s">
         <v>141</v>
@@ -4651,7 +4653,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B72" s="28" t="s">
         <v>142</v>
@@ -4671,7 +4673,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B73" s="28" t="s">
         <v>144</v>
@@ -4691,7 +4693,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B74" s="28" t="s">
         <v>350</v>
@@ -4711,7 +4713,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B75" s="28" t="s">
         <v>147</v>
@@ -4731,7 +4733,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B76" s="28" t="s">
         <v>149</v>
@@ -4751,7 +4753,7 @@
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B77" s="28" t="s">
         <v>151</v>
@@ -4771,7 +4773,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B78" s="28" t="s">
         <v>153</v>
@@ -4791,7 +4793,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B79" s="28" t="s">
         <v>155</v>
@@ -4811,7 +4813,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B80" s="28" t="s">
         <v>157</v>
@@ -4831,7 +4833,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B81" s="28" t="s">
         <v>158</v>
@@ -4851,7 +4853,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B82" s="28" t="s">
         <v>160</v>
@@ -4871,7 +4873,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B83" s="28" t="s">
         <v>162</v>
@@ -4891,7 +4893,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B84" s="28" t="s">
         <v>164</v>
@@ -4911,7 +4913,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B85" s="28" t="s">
         <v>166</v>
@@ -4931,7 +4933,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B86" s="28" t="s">
         <v>168</v>
@@ -4951,7 +4953,7 @@
     </row>
     <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B87" s="28" t="s">
         <v>170</v>
@@ -4971,7 +4973,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B88" s="28" t="s">
         <v>173</v>
@@ -4991,7 +4993,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B89" s="28" t="s">
         <v>175</v>
@@ -5011,7 +5013,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B90" s="28" t="s">
         <v>177</v>
@@ -5031,7 +5033,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B91" s="28" t="s">
         <v>179</v>
@@ -5051,7 +5053,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B92" s="28" t="s">
         <v>181</v>
@@ -5071,7 +5073,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B93" s="28" t="s">
         <v>183</v>
@@ -5091,7 +5093,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B94" s="28" t="s">
         <v>184</v>
@@ -5111,7 +5113,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B95" s="28" t="s">
         <v>186</v>
@@ -5131,7 +5133,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B96" s="28" t="s">
         <v>187</v>
@@ -5151,7 +5153,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B97" s="28" t="s">
         <v>189</v>
@@ -5171,7 +5173,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B98" s="28" t="s">
         <v>191</v>
@@ -5191,7 +5193,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B99" s="28" t="s">
         <v>193</v>
@@ -5211,7 +5213,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>194</v>
@@ -5231,7 +5233,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>196</v>
@@ -5251,7 +5253,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>351</v>
@@ -5271,7 +5273,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B103" s="28" t="s">
         <v>200</v>
@@ -5291,7 +5293,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B104" s="28" t="s">
         <v>202</v>
@@ -5311,7 +5313,7 @@
     </row>
     <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B105" s="28" t="s">
         <v>204</v>
@@ -5331,7 +5333,7 @@
     </row>
     <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B106" s="28" t="s">
         <v>206</v>
@@ -5351,7 +5353,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B107" s="28" t="s">
         <v>207</v>
@@ -5371,7 +5373,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B108" s="28" t="s">
         <v>209</v>
@@ -5391,7 +5393,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B109" s="28" t="s">
         <v>211</v>
@@ -5411,7 +5413,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B110" s="28" t="s">
         <v>212</v>
@@ -5431,7 +5433,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B111" s="28" t="s">
         <v>214</v>
@@ -5451,7 +5453,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B112" s="28" t="s">
         <v>216</v>
@@ -5471,7 +5473,7 @@
     </row>
     <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B113" s="28" t="s">
         <v>218</v>
@@ -5491,7 +5493,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B114" s="28" t="s">
         <v>220</v>
@@ -5511,7 +5513,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B115" s="28" t="s">
         <v>222</v>
@@ -5531,7 +5533,7 @@
     </row>
     <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B116" s="28" t="s">
         <v>223</v>
@@ -5551,7 +5553,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B117" s="28" t="s">
         <v>225</v>
@@ -5571,7 +5573,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B118" s="28" t="s">
         <v>227</v>
@@ -5591,7 +5593,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B119" s="28" t="s">
         <v>229</v>
@@ -5611,7 +5613,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B120" s="28" t="s">
         <v>231</v>
@@ -5631,7 +5633,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B121" s="28" t="s">
         <v>233</v>
@@ -5651,7 +5653,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B122" s="28" t="s">
         <v>235</v>
@@ -5671,7 +5673,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B123" s="28" t="s">
         <v>237</v>
@@ -5691,7 +5693,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B124" s="28" t="s">
         <v>239</v>
@@ -5711,7 +5713,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B125" s="28" t="s">
         <v>241</v>
@@ -5731,7 +5733,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B126" s="28" t="s">
         <v>243</v>
@@ -5751,7 +5753,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B127" s="28" t="s">
         <v>245</v>
@@ -5771,7 +5773,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B128" s="28" t="s">
         <v>247</v>
@@ -5791,7 +5793,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B129" s="28" t="s">
         <v>249</v>
@@ -5811,7 +5813,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B130" s="28" t="s">
         <v>251</v>
@@ -5831,7 +5833,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B131" s="28" t="s">
         <v>253</v>
@@ -5851,7 +5853,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B132" s="28" t="s">
         <v>255</v>
@@ -5871,7 +5873,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B133" s="28" t="s">
         <v>257</v>
@@ -5891,7 +5893,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B134" s="28" t="s">
         <v>259</v>
@@ -5911,7 +5913,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B135" s="28" t="s">
         <v>261</v>
@@ -5931,7 +5933,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B136" s="28" t="s">
         <v>263</v>
@@ -5951,7 +5953,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B137" s="28" t="s">
         <v>265</v>
@@ -5971,7 +5973,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B138" s="28" t="s">
         <v>267</v>
@@ -5991,7 +5993,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B139" s="28" t="s">
         <v>269</v>
@@ -6011,7 +6013,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B140" s="28" t="s">
         <v>271</v>
@@ -6031,7 +6033,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B141" s="28" t="s">
         <v>273</v>
@@ -6051,7 +6053,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B142" s="28" t="s">
         <v>275</v>
@@ -6071,7 +6073,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B143" s="28" t="s">
         <v>277</v>
@@ -6091,7 +6093,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B144" s="28" t="s">
         <v>279</v>
@@ -6111,7 +6113,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B145" s="28" t="s">
         <v>281</v>
@@ -6131,7 +6133,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B146" s="28" t="s">
         <v>283</v>
@@ -6151,7 +6153,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B147" s="28" t="s">
         <v>285</v>
@@ -6171,7 +6173,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B148" s="28" t="s">
         <v>287</v>
@@ -6191,7 +6193,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B149" s="28" t="s">
         <v>289</v>
@@ -6211,7 +6213,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B150" s="28" t="s">
         <v>291</v>
@@ -6231,7 +6233,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B151" s="28" t="s">
         <v>293</v>
@@ -6251,7 +6253,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B152" s="28" t="s">
         <v>295</v>
@@ -6271,7 +6273,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B153" s="28" t="s">
         <v>297</v>
@@ -6291,7 +6293,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B154" s="28" t="s">
         <v>299</v>
@@ -6311,7 +6313,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B155" s="28" t="s">
         <v>301</v>
@@ -6331,7 +6333,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B156" s="28" t="s">
         <v>303</v>
@@ -6351,7 +6353,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B157" s="28" t="s">
         <v>305</v>
@@ -6371,7 +6373,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B158" s="28" t="s">
         <v>307</v>
@@ -6391,7 +6393,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B159" s="28" t="s">
         <v>309</v>
@@ -6411,7 +6413,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B160" s="28" t="s">
         <v>311</v>
@@ -6431,7 +6433,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B161" s="28" t="s">
         <v>313</v>
@@ -6451,7 +6453,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B162" s="28" t="s">
         <v>315</v>
@@ -6471,7 +6473,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B163" s="28" t="s">
         <v>317</v>
@@ -6491,7 +6493,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B164" s="28" t="s">
         <v>319</v>
@@ -6511,7 +6513,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B165" s="28" t="s">
         <v>321</v>
@@ -6531,7 +6533,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B166" s="28" t="s">
         <v>323</v>
@@ -6551,7 +6553,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B167" s="28" t="s">
         <v>325</v>
@@ -6571,7 +6573,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B168" s="28" t="s">
         <v>327</v>
@@ -6591,7 +6593,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B169" s="28" t="s">
         <v>329</v>
@@ -6611,7 +6613,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B170" s="28" t="s">
         <v>331</v>
@@ -6631,7 +6633,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B171" s="28" t="s">
         <v>333</v>
@@ -6651,7 +6653,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B172" s="28" t="s">
         <v>335</v>
@@ -6671,7 +6673,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B173" s="28" t="s">
         <v>337</v>
@@ -6691,7 +6693,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B174" s="28" t="s">
         <v>339</v>
@@ -6711,7 +6713,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B175" s="28" t="s">
         <v>341</v>
@@ -6731,7 +6733,7 @@
     </row>
     <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B176" s="28" t="s">
         <v>343</v>
@@ -6751,7 +6753,7 @@
     </row>
     <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B177" s="28" t="s">
         <v>345</v>
@@ -6771,7 +6773,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B178" s="28" t="s">
         <v>346</v>
@@ -6791,7 +6793,7 @@
     </row>
     <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B179" s="28" t="s">
         <v>352</v>
@@ -6811,7 +6813,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B180" s="28" t="s">
         <v>354</v>
@@ -6831,7 +6833,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B181" s="28" t="s">
         <v>356</v>
@@ -6851,7 +6853,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B182" s="28" t="s">
         <v>357</v>
@@ -6871,7 +6873,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B183" s="28" t="s">
         <v>359</v>
@@ -6891,7 +6893,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B184" s="28" t="s">
         <v>361</v>
@@ -6911,7 +6913,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B185" s="28" t="s">
         <v>363</v>
@@ -6931,7 +6933,7 @@
     </row>
     <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B186" s="27" t="s">
         <v>365</v>
@@ -6951,7 +6953,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="6" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B187" s="27" t="s">
         <v>367</v>
@@ -6971,7 +6973,7 @@
     </row>
     <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B188" s="28" t="s">
         <v>369</v>
@@ -6991,7 +6993,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="6" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B189" s="28" t="s">
         <v>371</v>
@@ -7011,7 +7013,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B190" s="28" t="s">
         <v>373</v>
@@ -7031,7 +7033,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B191" s="28" t="s">
         <v>375</v>
@@ -7051,7 +7053,7 @@
     </row>
     <row r="192" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B192" s="28" t="s">
         <v>377</v>
@@ -7071,7 +7073,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B193" s="28" t="s">
         <v>379</v>
@@ -7091,7 +7093,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B194" s="28" t="s">
         <v>382</v>
@@ -7111,7 +7113,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B195" s="28" t="s">
         <v>383</v>
@@ -7131,7 +7133,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B196" s="28" t="s">
         <v>385</v>
@@ -7151,7 +7153,7 @@
     </row>
     <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B197" s="28" t="s">
         <v>387</v>
@@ -7171,7 +7173,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="6" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B198" s="28" t="s">
         <v>389</v>
@@ -7191,7 +7193,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B199" s="28" t="s">
         <v>391</v>
@@ -7211,7 +7213,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="6" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B200" s="28" t="s">
         <v>393</v>
@@ -7231,7 +7233,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B201" s="28" t="s">
         <v>395</v>
@@ -7251,7 +7253,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B202" s="28" t="s">
         <v>396</v>
@@ -7271,7 +7273,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="6" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B203" s="28" t="s">
         <v>397</v>
@@ -7291,7 +7293,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B204" s="28" t="s">
         <v>398</v>
@@ -7311,7 +7313,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B205" s="28" t="s">
         <v>399</v>
@@ -7331,7 +7333,7 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B206" s="28" t="s">
         <v>400</v>
@@ -7351,7 +7353,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="6" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B207" s="28" t="s">
         <v>401</v>
@@ -7371,7 +7373,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B208" s="28" t="s">
         <v>402</v>
@@ -7391,7 +7393,7 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B209" s="28" t="s">
         <v>403</v>
@@ -7411,7 +7413,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B210" s="28" t="s">
         <v>404</v>
@@ -7431,7 +7433,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B211" s="28" t="s">
         <v>405</v>
@@ -7451,7 +7453,7 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B212" s="28" t="s">
         <v>407</v>
@@ -7471,7 +7473,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B213" s="28" t="s">
         <v>409</v>
@@ -7491,7 +7493,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B214" s="28" t="s">
         <v>411</v>
@@ -7511,7 +7513,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B215" s="28" t="s">
         <v>413</v>
@@ -7531,7 +7533,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="6" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B216" s="28" t="s">
         <v>415</v>
@@ -7551,7 +7553,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B217" s="28" t="s">
         <v>417</v>
@@ -7571,7 +7573,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B218" s="28" t="s">
         <v>419</v>
@@ -7591,7 +7593,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B219" s="29" t="s">
         <v>422</v>
@@ -7611,7 +7613,7 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B220" s="29" t="s">
         <v>423</v>
@@ -7631,7 +7633,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B221" s="29" t="s">
         <v>424</v>
@@ -7651,7 +7653,7 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B222" s="29" t="s">
         <v>425</v>
@@ -7671,7 +7673,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B223" s="29" t="s">
         <v>426</v>
@@ -7691,7 +7693,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B224" s="29" t="s">
         <v>427</v>
@@ -7711,7 +7713,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B225" s="29" t="s">
         <v>428</v>
@@ -7731,7 +7733,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B226" s="30" t="s">
         <v>429</v>
@@ -7751,7 +7753,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B227" s="29" t="s">
         <v>430</v>
@@ -7771,7 +7773,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B228" s="29" t="s">
         <v>431</v>
@@ -7791,7 +7793,7 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B229" s="29" t="s">
         <v>432</v>
@@ -7811,7 +7813,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B230" s="29" t="s">
         <v>433</v>
@@ -7831,7 +7833,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="6" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B231" s="29" t="s">
         <v>434</v>
@@ -7851,7 +7853,7 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B232" s="29" t="s">
         <v>435</v>
@@ -7871,10 +7873,10 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="6" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B233" s="29" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>436</v>
@@ -7891,13 +7893,13 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B234" s="29" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D234" s="5" t="b">
         <v>1</v>
@@ -7911,13 +7913,13 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B235" s="29" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D235" s="5" t="b">
         <v>1</v>
@@ -7931,13 +7933,13 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B236" s="29" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D236" s="5" t="b">
         <v>1</v>
@@ -7951,10 +7953,10 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B237" s="30" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C237" s="20" t="s">
         <v>437</v>
@@ -7971,7 +7973,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B238" s="29" t="s">
         <v>438</v>
@@ -7991,7 +7993,7 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B239" s="30" t="s">
         <v>440</v>
@@ -8011,7 +8013,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B240" s="29" t="s">
         <v>442</v>
@@ -8031,7 +8033,7 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="6" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B241" s="29" t="s">
         <v>444</v>
@@ -8051,7 +8053,7 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B242" s="29" t="s">
         <v>446</v>
@@ -8071,7 +8073,7 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="6" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B243" s="29" t="s">
         <v>448</v>
@@ -8091,7 +8093,7 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B244" s="29" t="s">
         <v>450</v>
@@ -8111,7 +8113,7 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B245" s="29" t="s">
         <v>452</v>
@@ -8131,7 +8133,7 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B246" s="32" t="s">
         <v>454</v>
@@ -8151,13 +8153,13 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B247" s="29" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D247" s="5" t="b">
         <v>1</v>
@@ -8171,10 +8173,10 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B248" s="29" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>456</v>
@@ -8191,7 +8193,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="6" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B249" s="31" t="s">
         <v>463</v>
@@ -8211,7 +8213,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B250" s="31" t="s">
         <v>465</v>
@@ -8231,7 +8233,7 @@
     </row>
     <row r="251" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="6" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B251" s="31" t="s">
         <v>467</v>
@@ -8251,7 +8253,7 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B252" s="27" t="s">
         <v>468</v>
@@ -8271,7 +8273,7 @@
     </row>
     <row r="253" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" s="6" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B253" s="27" t="s">
         <v>470</v>
@@ -8291,13 +8293,13 @@
     </row>
     <row r="254" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="6" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B254" s="28" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C254" s="22" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D254" s="25" t="b">
         <v>1</v>
@@ -8311,13 +8313,13 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="6" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B255" s="28" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C255" s="22" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D255" s="25" t="b">
         <v>1</v>
@@ -8331,10 +8333,10 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B256" s="28" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C256" s="22" t="s">
         <v>539</v>
@@ -8351,10 +8353,10 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="6" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B257" s="28" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C257" s="23" t="s">
         <v>541</v>
@@ -8371,13 +8373,13 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="6" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B258" s="28" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C258" s="22" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D258" s="25" t="b">
         <v>1</v>
@@ -8391,10 +8393,10 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="6" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B259" s="28" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C259" s="24" t="s">
         <v>543</v>
@@ -8411,7 +8413,7 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B260" s="28" t="s">
         <v>562</v>
@@ -8431,7 +8433,7 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="6" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B261" s="28" t="s">
         <v>561</v>
@@ -8451,7 +8453,7 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="6" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B262" s="28" t="s">
         <v>477</v>
@@ -8471,7 +8473,7 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B263" s="28" t="s">
         <v>479</v>
@@ -8491,7 +8493,7 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="6" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B264" s="28" t="s">
         <v>480</v>
@@ -8511,7 +8513,7 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="6" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B265" s="28" t="s">
         <v>481</v>
@@ -8531,7 +8533,7 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="6" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B266" s="28" t="s">
         <v>482</v>
@@ -8551,7 +8553,7 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="6" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B267" s="28" t="s">
         <v>483</v>
@@ -8571,7 +8573,7 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="6" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B268" s="28" t="s">
         <v>484</v>
@@ -8591,7 +8593,7 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B269" s="28" t="s">
         <v>485</v>
@@ -8611,7 +8613,7 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B270" s="28" t="s">
         <v>486</v>
@@ -8631,7 +8633,7 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="6" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B271" s="28" t="s">
         <v>487</v>
@@ -8651,7 +8653,7 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B272" s="28" t="s">
         <v>488</v>
@@ -8671,7 +8673,7 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="6" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B273" s="28" t="s">
         <v>489</v>
@@ -8691,7 +8693,7 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B274" s="28" t="s">
         <v>490</v>
@@ -8711,7 +8713,7 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="6" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B275" s="28" t="s">
         <v>491</v>
@@ -8731,7 +8733,7 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="6" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B276" s="28" t="s">
         <v>493</v>
@@ -8751,7 +8753,7 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="6" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B277" s="28" t="s">
         <v>494</v>
@@ -8771,7 +8773,7 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B278" s="28" t="s">
         <v>495</v>
@@ -8791,7 +8793,7 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="6" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B279" s="28" t="s">
         <v>496</v>
@@ -8811,7 +8813,7 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B280" s="28" t="s">
         <v>497</v>
@@ -8831,7 +8833,7 @@
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B281" s="28" t="s">
         <v>498</v>
@@ -8851,7 +8853,7 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B282" s="28" t="s">
         <v>499</v>
@@ -8871,7 +8873,7 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B283" s="28" t="s">
         <v>500</v>
@@ -8891,7 +8893,7 @@
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B284" s="28" t="s">
         <v>501</v>
@@ -8911,7 +8913,7 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="6" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B285" s="28" t="s">
         <v>502</v>
@@ -8931,7 +8933,7 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="6" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B286" s="28" t="s">
         <v>503</v>
@@ -8951,7 +8953,7 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="6" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B287" s="28" t="s">
         <v>504</v>
@@ -8971,7 +8973,7 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="6" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B288" s="28" t="s">
         <v>505</v>
@@ -8991,7 +8993,7 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="6" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B289" s="28" t="s">
         <v>506</v>
@@ -9011,7 +9013,7 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B290" s="28" t="s">
         <v>507</v>
@@ -9031,7 +9033,7 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="6" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B291" s="28" t="s">
         <v>508</v>
@@ -9051,7 +9053,7 @@
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B292" s="28" t="s">
         <v>509</v>
@@ -9071,7 +9073,7 @@
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="6" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B293" s="28" t="s">
         <v>510</v>
@@ -9091,7 +9093,7 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B294" s="28" t="s">
         <v>511</v>
@@ -9111,7 +9113,7 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="6" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B295" s="28" t="s">
         <v>512</v>
@@ -9131,7 +9133,7 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="6" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B296" s="28" t="s">
         <v>513</v>
@@ -9151,7 +9153,7 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="6" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B297" s="28" t="s">
         <v>514</v>
@@ -9171,7 +9173,7 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B298" s="28" t="s">
         <v>515</v>
@@ -9191,7 +9193,7 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="6" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B299" s="28" t="s">
         <v>516</v>
@@ -9211,7 +9213,7 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B300" s="28" t="s">
         <v>517</v>
@@ -9231,7 +9233,7 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B301" s="28" t="s">
         <v>518</v>
@@ -9251,7 +9253,7 @@
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="6" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B302" s="28" t="s">
         <v>519</v>
@@ -9271,7 +9273,7 @@
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="6" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B303" s="28" t="s">
         <v>520</v>
@@ -9291,7 +9293,7 @@
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B304" s="28" t="s">
         <v>521</v>
@@ -9311,7 +9313,7 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="6" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B305" s="28" t="s">
         <v>522</v>
@@ -9331,7 +9333,7 @@
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B306" s="28" t="s">
         <v>523</v>
@@ -9351,7 +9353,7 @@
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B307" s="28" t="s">
         <v>524</v>
@@ -9371,7 +9373,7 @@
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B308" s="28" t="s">
         <v>525</v>
@@ -9391,7 +9393,7 @@
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="6" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B309" s="28" t="s">
         <v>526</v>
@@ -9411,7 +9413,7 @@
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="6" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B310" s="28" t="s">
         <v>527</v>
@@ -9431,7 +9433,7 @@
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B311" s="28" t="s">
         <v>528</v>
@@ -9451,7 +9453,7 @@
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B312" s="28" t="s">
         <v>529</v>
@@ -9471,7 +9473,7 @@
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="6" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B313" s="28" t="s">
         <v>530</v>
@@ -9491,7 +9493,7 @@
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="6" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B314" s="28" t="s">
         <v>531</v>
@@ -9511,7 +9513,7 @@
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="6" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B315" s="28" t="s">
         <v>532</v>
@@ -9531,7 +9533,7 @@
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B316" s="28" t="s">
         <v>533</v>
@@ -9551,7 +9553,7 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="6" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B317" s="28" t="s">
         <v>534</v>
@@ -9571,7 +9573,7 @@
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="6" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B318" s="28" t="s">
         <v>535</v>
@@ -9591,7 +9593,7 @@
     </row>
     <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="6" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B319" s="28" t="s">
         <v>536</v>
@@ -9611,7 +9613,7 @@
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B320" s="28" t="s">
         <v>559</v>

</xml_diff>

<commit_message>
Converting some regexs to TOMES Patterns.
</commit_message>
<xml_diff>
--- a/dictionaries/TOMES_Entity_Dictionary.xlsx
+++ b/dictionaries/TOMES_Entity_Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="20400" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="20400" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -27,40 +27,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Nitin</author>
-  </authors>
-  <commentList>
-    <comment ref="B255" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Nitin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Change this to TOMES.EMAIL and add why it's not PII.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="904">
   <si>
@@ -1678,9 +1644,6 @@
     <t>PII.bank_account_number</t>
   </si>
   <si>
-    <t>PII.email_address</t>
-  </si>
-  <si>
     <t>United States passport number or a United States visa number.</t>
   </si>
   <si>
@@ -1744,21 +1707,12 @@
     <t>(http|https|ftp){1}(://)([0-9a-zA-Z]){1,63}(\.|@|:)([^\s]){1,2000}</t>
   </si>
   <si>
-    <t>A Uniform Resource Locator or File Transfer Protocal string reference.</t>
-  </si>
-  <si>
-    <t>(?!000)([0-6][0-9]{2}|7([0-6][0-9]{1}|7[012]))([\s{1}-]){0,1}(?!00)[0-9]{2}\3(?!0000)[0-9]{4}</t>
-  </si>
-  <si>
     <t>[0]{4}[0-9]{8}</t>
   </si>
   <si>
     <t>[0-9]{2}-[0-9]{7}([a-zA-Z]|[0-9]{3}){0,1}</t>
   </si>
   <si>
-    <t>[0-9]{4}[\s|-][0-9]{4}[\s|-][0-9]{4}[\s|-]{0,1}[0-9]{4}</t>
-  </si>
-  <si>
     <t>[0-9]{8}</t>
   </si>
   <si>
@@ -1771,30 +1725,6 @@
     <t>Checking and savings account numbers, with or without routing numbers. Those with routing numbers are more likely to be actual account numbers.</t>
   </si>
   <si>
-    <t>([1-9]|[1-5][0-9])\s(USC|U\.S\.C)(\s§{1,2}){0,1}\s[1-9][0-9]{0,2}(-[1-9][0-9]{0,3}){0,1}</t>
-  </si>
-  <si>
-    <t>((?i)Senate\sBill(?-i)|S|SB|S\.\s{0,1}B\.)\s{0,1}[0-9]{1,4}</t>
-  </si>
-  <si>
-    <t>([1-9]|[1-5][0-9])\s(CFR|C\.F\.R)(\s§){0,1}\s[0-9]{1,4}(\.[1-9]{1,4}){0,1}</t>
-  </si>
-  <si>
-    <t>([1-9]|[1-3][0-9])[A-Z]{0,1}\s(N\.C\.\sAdmin\.\sCode|NC\sAdmin\.\sCode|NCAC)\s[1-9][0-9]{0,1}[A-Z]\.[0-9]{1,4}</t>
-  </si>
-  <si>
-    <t>((?i)House\sBill(?-i)\s|H|HB\s{0,1}|H\.\s{0,1}B\.\s)[0-9]{1,4}</t>
-  </si>
-  <si>
-    <t>((?i)General\sStatute(?-i)\s|GS\s{0,1}|G\.\s{0,1}S\.\s)(§\s{0,1}){0,1}[12][0-9]{0,2}[a-zA-Z]{0,1}</t>
-  </si>
-  <si>
-    <t>(Executive\sOrder\s|Executive\sOrder\sNo\.\s|EO\s{0,1}|E\.\s{0,1}O\.\s)[0-9]{1,3}</t>
-  </si>
-  <si>
-    <t>((0[0-9])|(1[0-2])|(2[1-9])|(3[0-2])|(6[1-9])|(7[0-2])|80)[0-9]{2}-{0,1}[0-9]{4}-{0,1}[0-9](\s|-)[0-9]{6,17}</t>
-  </si>
-  <si>
     <t>North Carolina Senate Bill citation.</t>
   </si>
   <si>
@@ -1807,9 +1737,6 @@
     <t>North Carolina Executive Order citation.</t>
   </si>
   <si>
-    <t>An electronic mailing address.</t>
-  </si>
-  <si>
     <t>Credit or debit card number.</t>
   </si>
   <si>
@@ -2774,13 +2701,52 @@
   </si>
   <si>
     <t>Patterns using regular expressions and TOMES Patterns are highlighted in green via Conditional Formatting.</t>
+  </si>
+  <si>
+    <t>TOMES.email_address</t>
+  </si>
+  <si>
+    <t>An electronic mailing address. Note, in North Carolina email addresses fall under the legal definition of PII in G.S. 14-113.20, G.S. 132 exempts them from the confidentiality requirements.</t>
+  </si>
+  <si>
+    <t>A Uniform Resource Locator (URL) or File Transfer Protocal (FTP) string reference.</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"((0[0-9])|(1[0-2])|(2[1-9])|(3[0-2])|(6[1-9])|(7[0-2])|80)[0-9]{2}-{0,1}[0-9]{4}-{0,1}[0-9]"}, {" ", "-"}, {"[0-9]{6,17}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"(?!000)"}, {"([0-6][0-9]{2}|7([0-6][0-9]{1}|7[012]))"}, {" ", "-"}, {"(?!00)"}, {"[0-9]{2}"}, {" ", "-"}, {"(?!0000)"}, {"[0-9]{4}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"[0-9]{4}"}, {" ", "-"}, {"[0-9]{4}"}, {" ", "-"}, {"[0-9]{4}"}, {"", " ", "-"}, {"[0-9]{4}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"([1-9]|[1-5][0-9])"}, {" "}, {"(USC|U\.S\.C)"}, {"", " "}, {"(§{1,2}){0,1}"}, {" "}, {"[1-9][0-9]{0,2}(-[1-9][0-9]{0,3}){0,1}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"([1-9]|[1-3][0-9])[A-Z]{0,1}"}, {" "}, {"N.C. Admin Code", "NC Admin Code", "NCAC"}, {" "}, {"[1-9][0-9]{0,1}[A-Z]\.[0-9]{1,4}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"(?i)Senate(?-i) (?i)Bill(?-i)", "S", "SB", "S.B.", "S. B."}, {"", " "}, {"[0-9]{1,4}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"(?i)House(?-i) (?i)Bill(?-i)", "H", "HB", "H. B.", "H.B."}, {"" , " "}, {"[0-9]{1,4}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"(?i)General(?-i) (?i)Statute(?-i)", "GS", "G. S.", "G.S."}, {" "}, {"", "§", "§ "}, {"[12][0-9]{0,2}[a-zA-Z]{0,1}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"(?i)Executive(?-i) (?i)Order(?-i)", "(?i)Executive(?-i) (?i)Order(?-i) (?i)No(?-i).", "EO", "E. O."}, {" "}, {"[0-9]{1,3}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"([1-9]|[1-5][0-9])"}, {" "}, {"(CFR|C\.F\.R)"}, {"", " §"}, {" "}, {"[0-9]{1,4}(\.[1-9]{1,4}){0,1}"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2802,19 +2768,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2932,11 +2885,11 @@
   <dxfs count="3">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2952,11 +2905,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3246,12 +3199,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>902</v>
+        <v>889</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>903</v>
+        <v>890</v>
       </c>
     </row>
   </sheetData>
@@ -3260,12 +3213,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C260" sqref="C260"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3300,7 +3253,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>583</v>
+        <v>570</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>5</v>
@@ -3320,7 +3273,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>14</v>
@@ -3340,7 +3293,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>6</v>
@@ -3360,7 +3313,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>7</v>
@@ -3380,7 +3333,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>8</v>
@@ -3400,7 +3353,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="B7" s="28" t="s">
         <v>9</v>
@@ -3420,7 +3373,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>10</v>
@@ -3440,7 +3393,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>11</v>
@@ -3460,7 +3413,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>16</v>
@@ -3480,7 +3433,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>15</v>
@@ -3500,7 +3453,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>26</v>
@@ -3520,7 +3473,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>29</v>
@@ -3540,7 +3493,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>30</v>
@@ -3560,7 +3513,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>31</v>
@@ -3580,7 +3533,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>597</v>
+        <v>584</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>32</v>
@@ -3600,7 +3553,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>33</v>
@@ -3620,7 +3573,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>34</v>
@@ -3640,7 +3593,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>35</v>
@@ -3660,7 +3613,7 @@
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="B20" s="28" t="s">
         <v>36</v>
@@ -3680,7 +3633,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>38</v>
@@ -3700,7 +3653,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>40</v>
@@ -3720,7 +3673,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>42</v>
@@ -3740,7 +3693,7 @@
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>44</v>
@@ -3760,7 +3713,7 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="B25" s="28" t="s">
         <v>46</v>
@@ -3780,7 +3733,7 @@
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>48</v>
@@ -3800,7 +3753,7 @@
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>50</v>
@@ -3820,7 +3773,7 @@
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>52</v>
@@ -3840,7 +3793,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>53</v>
@@ -3860,7 +3813,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>55</v>
@@ -3880,7 +3833,7 @@
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="B31" s="28" t="s">
         <v>56</v>
@@ -3900,7 +3853,7 @@
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>58</v>
@@ -3920,7 +3873,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
       <c r="B33" s="28" t="s">
         <v>60</v>
@@ -3940,7 +3893,7 @@
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="B34" s="28" t="s">
         <v>62</v>
@@ -3960,7 +3913,7 @@
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="B35" s="28" t="s">
         <v>64</v>
@@ -3980,7 +3933,7 @@
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="B36" s="28" t="s">
         <v>66</v>
@@ -4000,7 +3953,7 @@
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="B37" s="28" t="s">
         <v>68</v>
@@ -4020,7 +3973,7 @@
     </row>
     <row r="38" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>78</v>
@@ -4040,7 +3993,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="B39" s="28" t="s">
         <v>80</v>
@@ -4060,7 +4013,7 @@
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="B40" s="28" t="s">
         <v>81</v>
@@ -4080,7 +4033,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="B41" s="28" t="s">
         <v>82</v>
@@ -4100,7 +4053,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="B42" s="28" t="s">
         <v>83</v>
@@ -4120,7 +4073,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="B43" s="28" t="s">
         <v>84</v>
@@ -4140,7 +4093,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
       <c r="B44" s="28" t="s">
         <v>85</v>
@@ -4160,7 +4113,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>626</v>
+        <v>613</v>
       </c>
       <c r="B45" s="28" t="s">
         <v>86</v>
@@ -4180,7 +4133,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>627</v>
+        <v>614</v>
       </c>
       <c r="B46" s="28" t="s">
         <v>87</v>
@@ -4200,7 +4153,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="B47" s="28" t="s">
         <v>88</v>
@@ -4220,7 +4173,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
       <c r="B48" s="28" t="s">
         <v>89</v>
@@ -4240,7 +4193,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="B49" s="28" t="s">
         <v>90</v>
@@ -4260,7 +4213,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
       <c r="B50" s="28" t="s">
         <v>91</v>
@@ -4280,7 +4233,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>632</v>
+        <v>619</v>
       </c>
       <c r="B51" s="28" t="s">
         <v>92</v>
@@ -4300,7 +4253,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="B52" s="28" t="s">
         <v>93</v>
@@ -4320,7 +4273,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="B53" s="28" t="s">
         <v>94</v>
@@ -4340,7 +4293,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>635</v>
+        <v>622</v>
       </c>
       <c r="B54" s="28" t="s">
         <v>95</v>
@@ -4360,7 +4313,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="B55" s="29" t="s">
         <v>115</v>
@@ -4380,7 +4333,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="B56" s="28" t="s">
         <v>117</v>
@@ -4400,7 +4353,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="B57" s="28" t="s">
         <v>119</v>
@@ -4420,7 +4373,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="B58" s="28" t="s">
         <v>120</v>
@@ -4440,7 +4393,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>640</v>
+        <v>627</v>
       </c>
       <c r="B59" s="28" t="s">
         <v>122</v>
@@ -4460,7 +4413,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>641</v>
+        <v>628</v>
       </c>
       <c r="B60" s="28" t="s">
         <v>124</v>
@@ -4480,7 +4433,7 @@
     </row>
     <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>642</v>
+        <v>629</v>
       </c>
       <c r="B61" s="28" t="s">
         <v>126</v>
@@ -4500,7 +4453,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>643</v>
+        <v>630</v>
       </c>
       <c r="B62" s="28" t="s">
         <v>128</v>
@@ -4520,7 +4473,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>644</v>
+        <v>631</v>
       </c>
       <c r="B63" s="28" t="s">
         <v>349</v>
@@ -4540,7 +4493,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>645</v>
+        <v>632</v>
       </c>
       <c r="B64" s="28" t="s">
         <v>131</v>
@@ -4560,7 +4513,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="B65" s="28" t="s">
         <v>133</v>
@@ -4580,7 +4533,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>647</v>
+        <v>634</v>
       </c>
       <c r="B66" s="28" t="s">
         <v>134</v>
@@ -4600,7 +4553,7 @@
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>648</v>
+        <v>635</v>
       </c>
       <c r="B67" s="28" t="s">
         <v>135</v>
@@ -4620,7 +4573,7 @@
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>649</v>
+        <v>636</v>
       </c>
       <c r="B68" s="28" t="s">
         <v>136</v>
@@ -4640,7 +4593,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>650</v>
+        <v>637</v>
       </c>
       <c r="B69" s="28" t="s">
         <v>137</v>
@@ -4660,7 +4613,7 @@
     </row>
     <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>651</v>
+        <v>638</v>
       </c>
       <c r="B70" s="28" t="s">
         <v>139</v>
@@ -4680,7 +4633,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="B71" s="28" t="s">
         <v>141</v>
@@ -4700,7 +4653,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>653</v>
+        <v>640</v>
       </c>
       <c r="B72" s="28" t="s">
         <v>142</v>
@@ -4720,7 +4673,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>654</v>
+        <v>641</v>
       </c>
       <c r="B73" s="28" t="s">
         <v>144</v>
@@ -4740,7 +4693,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>655</v>
+        <v>642</v>
       </c>
       <c r="B74" s="28" t="s">
         <v>350</v>
@@ -4760,7 +4713,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>656</v>
+        <v>643</v>
       </c>
       <c r="B75" s="28" t="s">
         <v>147</v>
@@ -4780,7 +4733,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>657</v>
+        <v>644</v>
       </c>
       <c r="B76" s="28" t="s">
         <v>149</v>
@@ -4800,7 +4753,7 @@
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>658</v>
+        <v>645</v>
       </c>
       <c r="B77" s="28" t="s">
         <v>151</v>
@@ -4820,7 +4773,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B78" s="28" t="s">
         <v>153</v>
@@ -4840,7 +4793,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>660</v>
+        <v>647</v>
       </c>
       <c r="B79" s="28" t="s">
         <v>155</v>
@@ -4860,7 +4813,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>661</v>
+        <v>648</v>
       </c>
       <c r="B80" s="28" t="s">
         <v>157</v>
@@ -4880,7 +4833,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>662</v>
+        <v>649</v>
       </c>
       <c r="B81" s="28" t="s">
         <v>158</v>
@@ -4900,7 +4853,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>663</v>
+        <v>650</v>
       </c>
       <c r="B82" s="28" t="s">
         <v>160</v>
@@ -4920,7 +4873,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>664</v>
+        <v>651</v>
       </c>
       <c r="B83" s="28" t="s">
         <v>162</v>
@@ -4940,7 +4893,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>665</v>
+        <v>652</v>
       </c>
       <c r="B84" s="28" t="s">
         <v>164</v>
@@ -4960,7 +4913,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
       <c r="B85" s="28" t="s">
         <v>166</v>
@@ -4980,7 +4933,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>667</v>
+        <v>654</v>
       </c>
       <c r="B86" s="28" t="s">
         <v>168</v>
@@ -5000,7 +4953,7 @@
     </row>
     <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>668</v>
+        <v>655</v>
       </c>
       <c r="B87" s="28" t="s">
         <v>170</v>
@@ -5020,7 +4973,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>669</v>
+        <v>656</v>
       </c>
       <c r="B88" s="28" t="s">
         <v>173</v>
@@ -5040,7 +4993,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>670</v>
+        <v>657</v>
       </c>
       <c r="B89" s="28" t="s">
         <v>175</v>
@@ -5060,7 +5013,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="B90" s="28" t="s">
         <v>177</v>
@@ -5080,7 +5033,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="B91" s="28" t="s">
         <v>179</v>
@@ -5100,7 +5053,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
       <c r="B92" s="28" t="s">
         <v>181</v>
@@ -5120,7 +5073,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="B93" s="28" t="s">
         <v>183</v>
@@ -5140,7 +5093,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
       <c r="B94" s="28" t="s">
         <v>184</v>
@@ -5160,7 +5113,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
       <c r="B95" s="28" t="s">
         <v>186</v>
@@ -5180,7 +5133,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>677</v>
+        <v>664</v>
       </c>
       <c r="B96" s="28" t="s">
         <v>187</v>
@@ -5200,7 +5153,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>678</v>
+        <v>665</v>
       </c>
       <c r="B97" s="28" t="s">
         <v>189</v>
@@ -5220,7 +5173,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>679</v>
+        <v>666</v>
       </c>
       <c r="B98" s="28" t="s">
         <v>191</v>
@@ -5240,7 +5193,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>680</v>
+        <v>667</v>
       </c>
       <c r="B99" s="28" t="s">
         <v>193</v>
@@ -5260,7 +5213,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>681</v>
+        <v>668</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>194</v>
@@ -5280,7 +5233,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>682</v>
+        <v>669</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>196</v>
@@ -5300,7 +5253,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>683</v>
+        <v>670</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>351</v>
@@ -5320,7 +5273,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>684</v>
+        <v>671</v>
       </c>
       <c r="B103" s="28" t="s">
         <v>200</v>
@@ -5340,7 +5293,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>685</v>
+        <v>672</v>
       </c>
       <c r="B104" s="28" t="s">
         <v>202</v>
@@ -5360,7 +5313,7 @@
     </row>
     <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>686</v>
+        <v>673</v>
       </c>
       <c r="B105" s="28" t="s">
         <v>204</v>
@@ -5380,7 +5333,7 @@
     </row>
     <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
       <c r="B106" s="28" t="s">
         <v>206</v>
@@ -5400,7 +5353,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>688</v>
+        <v>675</v>
       </c>
       <c r="B107" s="28" t="s">
         <v>207</v>
@@ -5420,7 +5373,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>689</v>
+        <v>676</v>
       </c>
       <c r="B108" s="28" t="s">
         <v>209</v>
@@ -5440,7 +5393,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="B109" s="28" t="s">
         <v>211</v>
@@ -5460,7 +5413,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
       <c r="B110" s="28" t="s">
         <v>212</v>
@@ -5480,7 +5433,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
       <c r="B111" s="28" t="s">
         <v>214</v>
@@ -5500,7 +5453,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="B112" s="28" t="s">
         <v>216</v>
@@ -5520,7 +5473,7 @@
     </row>
     <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>694</v>
+        <v>681</v>
       </c>
       <c r="B113" s="28" t="s">
         <v>218</v>
@@ -5540,7 +5493,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>695</v>
+        <v>682</v>
       </c>
       <c r="B114" s="28" t="s">
         <v>220</v>
@@ -5560,7 +5513,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>696</v>
+        <v>683</v>
       </c>
       <c r="B115" s="28" t="s">
         <v>222</v>
@@ -5580,7 +5533,7 @@
     </row>
     <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>697</v>
+        <v>684</v>
       </c>
       <c r="B116" s="28" t="s">
         <v>223</v>
@@ -5600,7 +5553,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
       <c r="B117" s="28" t="s">
         <v>225</v>
@@ -5620,7 +5573,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="B118" s="28" t="s">
         <v>227</v>
@@ -5640,7 +5593,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
       <c r="B119" s="28" t="s">
         <v>229</v>
@@ -5660,7 +5613,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="B120" s="28" t="s">
         <v>231</v>
@@ -5680,7 +5633,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
       <c r="B121" s="28" t="s">
         <v>233</v>
@@ -5700,7 +5653,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
       <c r="B122" s="28" t="s">
         <v>235</v>
@@ -5720,7 +5673,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>704</v>
+        <v>691</v>
       </c>
       <c r="B123" s="28" t="s">
         <v>237</v>
@@ -5740,7 +5693,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>705</v>
+        <v>692</v>
       </c>
       <c r="B124" s="28" t="s">
         <v>239</v>
@@ -5760,7 +5713,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>706</v>
+        <v>693</v>
       </c>
       <c r="B125" s="28" t="s">
         <v>241</v>
@@ -5780,7 +5733,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>707</v>
+        <v>694</v>
       </c>
       <c r="B126" s="28" t="s">
         <v>243</v>
@@ -5800,7 +5753,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>708</v>
+        <v>695</v>
       </c>
       <c r="B127" s="28" t="s">
         <v>245</v>
@@ -5820,7 +5773,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>709</v>
+        <v>696</v>
       </c>
       <c r="B128" s="28" t="s">
         <v>247</v>
@@ -5840,7 +5793,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
-        <v>710</v>
+        <v>697</v>
       </c>
       <c r="B129" s="28" t="s">
         <v>249</v>
@@ -5860,7 +5813,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
-        <v>711</v>
+        <v>698</v>
       </c>
       <c r="B130" s="28" t="s">
         <v>251</v>
@@ -5880,7 +5833,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
-        <v>712</v>
+        <v>699</v>
       </c>
       <c r="B131" s="28" t="s">
         <v>253</v>
@@ -5900,7 +5853,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
-        <v>713</v>
+        <v>700</v>
       </c>
       <c r="B132" s="28" t="s">
         <v>255</v>
@@ -5920,7 +5873,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>714</v>
+        <v>701</v>
       </c>
       <c r="B133" s="28" t="s">
         <v>257</v>
@@ -5940,7 +5893,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>715</v>
+        <v>702</v>
       </c>
       <c r="B134" s="28" t="s">
         <v>259</v>
@@ -5960,7 +5913,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
       <c r="B135" s="28" t="s">
         <v>261</v>
@@ -5980,7 +5933,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="B136" s="28" t="s">
         <v>263</v>
@@ -6000,7 +5953,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>718</v>
+        <v>705</v>
       </c>
       <c r="B137" s="28" t="s">
         <v>265</v>
@@ -6020,7 +5973,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
-        <v>719</v>
+        <v>706</v>
       </c>
       <c r="B138" s="28" t="s">
         <v>267</v>
@@ -6040,7 +5993,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>720</v>
+        <v>707</v>
       </c>
       <c r="B139" s="28" t="s">
         <v>269</v>
@@ -6060,7 +6013,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>721</v>
+        <v>708</v>
       </c>
       <c r="B140" s="28" t="s">
         <v>271</v>
@@ -6080,7 +6033,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
       <c r="B141" s="28" t="s">
         <v>273</v>
@@ -6100,7 +6053,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
       <c r="B142" s="28" t="s">
         <v>275</v>
@@ -6120,7 +6073,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>724</v>
+        <v>711</v>
       </c>
       <c r="B143" s="28" t="s">
         <v>277</v>
@@ -6140,7 +6093,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>725</v>
+        <v>712</v>
       </c>
       <c r="B144" s="28" t="s">
         <v>279</v>
@@ -6160,7 +6113,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
-        <v>726</v>
+        <v>713</v>
       </c>
       <c r="B145" s="28" t="s">
         <v>281</v>
@@ -6180,7 +6133,7 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
-        <v>727</v>
+        <v>714</v>
       </c>
       <c r="B146" s="28" t="s">
         <v>283</v>
@@ -6200,7 +6153,7 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
-        <v>728</v>
+        <v>715</v>
       </c>
       <c r="B147" s="28" t="s">
         <v>285</v>
@@ -6220,7 +6173,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
-        <v>729</v>
+        <v>716</v>
       </c>
       <c r="B148" s="28" t="s">
         <v>287</v>
@@ -6240,7 +6193,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
-        <v>730</v>
+        <v>717</v>
       </c>
       <c r="B149" s="28" t="s">
         <v>289</v>
@@ -6260,7 +6213,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="B150" s="28" t="s">
         <v>291</v>
@@ -6280,7 +6233,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
-        <v>732</v>
+        <v>719</v>
       </c>
       <c r="B151" s="28" t="s">
         <v>293</v>
@@ -6300,7 +6253,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
-        <v>733</v>
+        <v>720</v>
       </c>
       <c r="B152" s="28" t="s">
         <v>295</v>
@@ -6320,7 +6273,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
-        <v>734</v>
+        <v>721</v>
       </c>
       <c r="B153" s="28" t="s">
         <v>297</v>
@@ -6340,7 +6293,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
-        <v>735</v>
+        <v>722</v>
       </c>
       <c r="B154" s="28" t="s">
         <v>299</v>
@@ -6360,7 +6313,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
       <c r="B155" s="28" t="s">
         <v>301</v>
@@ -6380,7 +6333,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
-        <v>737</v>
+        <v>724</v>
       </c>
       <c r="B156" s="28" t="s">
         <v>303</v>
@@ -6400,7 +6353,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
-        <v>738</v>
+        <v>725</v>
       </c>
       <c r="B157" s="28" t="s">
         <v>305</v>
@@ -6420,7 +6373,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
-        <v>739</v>
+        <v>726</v>
       </c>
       <c r="B158" s="28" t="s">
         <v>307</v>
@@ -6440,7 +6393,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
       <c r="B159" s="28" t="s">
         <v>309</v>
@@ -6460,7 +6413,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
       <c r="B160" s="28" t="s">
         <v>311</v>
@@ -6480,7 +6433,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
-        <v>742</v>
+        <v>729</v>
       </c>
       <c r="B161" s="28" t="s">
         <v>313</v>
@@ -6500,7 +6453,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
-        <v>743</v>
+        <v>730</v>
       </c>
       <c r="B162" s="28" t="s">
         <v>315</v>
@@ -6520,7 +6473,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
-        <v>744</v>
+        <v>731</v>
       </c>
       <c r="B163" s="28" t="s">
         <v>317</v>
@@ -6540,7 +6493,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
-        <v>745</v>
+        <v>732</v>
       </c>
       <c r="B164" s="28" t="s">
         <v>319</v>
@@ -6560,7 +6513,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
-        <v>746</v>
+        <v>733</v>
       </c>
       <c r="B165" s="28" t="s">
         <v>321</v>
@@ -6580,7 +6533,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
-        <v>747</v>
+        <v>734</v>
       </c>
       <c r="B166" s="28" t="s">
         <v>323</v>
@@ -6600,7 +6553,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
-        <v>748</v>
+        <v>735</v>
       </c>
       <c r="B167" s="28" t="s">
         <v>325</v>
@@ -6620,7 +6573,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
-        <v>749</v>
+        <v>736</v>
       </c>
       <c r="B168" s="28" t="s">
         <v>327</v>
@@ -6640,7 +6593,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>750</v>
+        <v>737</v>
       </c>
       <c r="B169" s="28" t="s">
         <v>329</v>
@@ -6660,7 +6613,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>751</v>
+        <v>738</v>
       </c>
       <c r="B170" s="28" t="s">
         <v>331</v>
@@ -6680,7 +6633,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>752</v>
+        <v>739</v>
       </c>
       <c r="B171" s="28" t="s">
         <v>333</v>
@@ -6700,7 +6653,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>753</v>
+        <v>740</v>
       </c>
       <c r="B172" s="28" t="s">
         <v>335</v>
@@ -6720,7 +6673,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>754</v>
+        <v>741</v>
       </c>
       <c r="B173" s="28" t="s">
         <v>337</v>
@@ -6740,7 +6693,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
-        <v>755</v>
+        <v>742</v>
       </c>
       <c r="B174" s="28" t="s">
         <v>339</v>
@@ -6760,7 +6713,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
       <c r="B175" s="28" t="s">
         <v>341</v>
@@ -6780,7 +6733,7 @@
     </row>
     <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>757</v>
+        <v>744</v>
       </c>
       <c r="B176" s="28" t="s">
         <v>343</v>
@@ -6800,7 +6753,7 @@
     </row>
     <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
-        <v>758</v>
+        <v>745</v>
       </c>
       <c r="B177" s="28" t="s">
         <v>345</v>
@@ -6820,7 +6773,7 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
-        <v>759</v>
+        <v>746</v>
       </c>
       <c r="B178" s="28" t="s">
         <v>346</v>
@@ -6840,7 +6793,7 @@
     </row>
     <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
-        <v>760</v>
+        <v>747</v>
       </c>
       <c r="B179" s="28" t="s">
         <v>352</v>
@@ -6860,7 +6813,7 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
-        <v>761</v>
+        <v>748</v>
       </c>
       <c r="B180" s="28" t="s">
         <v>354</v>
@@ -6880,7 +6833,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
-        <v>762</v>
+        <v>749</v>
       </c>
       <c r="B181" s="28" t="s">
         <v>356</v>
@@ -6900,7 +6853,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
-        <v>763</v>
+        <v>750</v>
       </c>
       <c r="B182" s="28" t="s">
         <v>357</v>
@@ -6920,7 +6873,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
-        <v>764</v>
+        <v>751</v>
       </c>
       <c r="B183" s="28" t="s">
         <v>359</v>
@@ -6940,7 +6893,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
-        <v>765</v>
+        <v>752</v>
       </c>
       <c r="B184" s="28" t="s">
         <v>361</v>
@@ -6960,7 +6913,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
-        <v>766</v>
+        <v>753</v>
       </c>
       <c r="B185" s="28" t="s">
         <v>363</v>
@@ -6980,7 +6933,7 @@
     </row>
     <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
-        <v>767</v>
+        <v>754</v>
       </c>
       <c r="B186" s="27" t="s">
         <v>365</v>
@@ -7000,7 +6953,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="6" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="B187" s="27" t="s">
         <v>367</v>
@@ -7020,7 +6973,7 @@
     </row>
     <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="B188" s="28" t="s">
         <v>369</v>
@@ -7040,7 +6993,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="6" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="B189" s="28" t="s">
         <v>371</v>
@@ -7060,7 +7013,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="B190" s="28" t="s">
         <v>373</v>
@@ -7080,7 +7033,7 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="B191" s="28" t="s">
         <v>375</v>
@@ -7100,7 +7053,7 @@
     </row>
     <row r="192" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
-        <v>773</v>
+        <v>760</v>
       </c>
       <c r="B192" s="28" t="s">
         <v>377</v>
@@ -7120,7 +7073,7 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
-        <v>774</v>
+        <v>761</v>
       </c>
       <c r="B193" s="28" t="s">
         <v>379</v>
@@ -7140,7 +7093,7 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
-        <v>775</v>
+        <v>762</v>
       </c>
       <c r="B194" s="28" t="s">
         <v>382</v>
@@ -7160,7 +7113,7 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
-        <v>776</v>
+        <v>763</v>
       </c>
       <c r="B195" s="28" t="s">
         <v>383</v>
@@ -7180,7 +7133,7 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
-        <v>777</v>
+        <v>764</v>
       </c>
       <c r="B196" s="28" t="s">
         <v>385</v>
@@ -7200,7 +7153,7 @@
     </row>
     <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
-        <v>778</v>
+        <v>765</v>
       </c>
       <c r="B197" s="28" t="s">
         <v>387</v>
@@ -7220,7 +7173,7 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="6" t="s">
-        <v>779</v>
+        <v>766</v>
       </c>
       <c r="B198" s="28" t="s">
         <v>389</v>
@@ -7240,7 +7193,7 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
-        <v>780</v>
+        <v>767</v>
       </c>
       <c r="B199" s="28" t="s">
         <v>391</v>
@@ -7260,7 +7213,7 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="6" t="s">
-        <v>781</v>
+        <v>768</v>
       </c>
       <c r="B200" s="28" t="s">
         <v>393</v>
@@ -7280,7 +7233,7 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
-        <v>782</v>
+        <v>769</v>
       </c>
       <c r="B201" s="28" t="s">
         <v>395</v>
@@ -7300,7 +7253,7 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
-        <v>783</v>
+        <v>770</v>
       </c>
       <c r="B202" s="28" t="s">
         <v>396</v>
@@ -7320,7 +7273,7 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="6" t="s">
-        <v>784</v>
+        <v>771</v>
       </c>
       <c r="B203" s="28" t="s">
         <v>397</v>
@@ -7340,7 +7293,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
-        <v>785</v>
+        <v>772</v>
       </c>
       <c r="B204" s="28" t="s">
         <v>398</v>
@@ -7360,7 +7313,7 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
-        <v>786</v>
+        <v>773</v>
       </c>
       <c r="B205" s="28" t="s">
         <v>399</v>
@@ -7380,7 +7333,7 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
-        <v>787</v>
+        <v>774</v>
       </c>
       <c r="B206" s="28" t="s">
         <v>400</v>
@@ -7400,7 +7353,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="6" t="s">
-        <v>788</v>
+        <v>775</v>
       </c>
       <c r="B207" s="28" t="s">
         <v>401</v>
@@ -7420,7 +7373,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
-        <v>789</v>
+        <v>776</v>
       </c>
       <c r="B208" s="28" t="s">
         <v>402</v>
@@ -7440,7 +7393,7 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
-        <v>790</v>
+        <v>777</v>
       </c>
       <c r="B209" s="28" t="s">
         <v>403</v>
@@ -7460,7 +7413,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
-        <v>791</v>
+        <v>778</v>
       </c>
       <c r="B210" s="28" t="s">
         <v>404</v>
@@ -7480,7 +7433,7 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
-        <v>792</v>
+        <v>779</v>
       </c>
       <c r="B211" s="28" t="s">
         <v>405</v>
@@ -7500,7 +7453,7 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
-        <v>793</v>
+        <v>780</v>
       </c>
       <c r="B212" s="28" t="s">
         <v>407</v>
@@ -7520,7 +7473,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
-        <v>794</v>
+        <v>781</v>
       </c>
       <c r="B213" s="28" t="s">
         <v>409</v>
@@ -7540,7 +7493,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
-        <v>795</v>
+        <v>782</v>
       </c>
       <c r="B214" s="28" t="s">
         <v>411</v>
@@ -7560,7 +7513,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
       <c r="B215" s="28" t="s">
         <v>413</v>
@@ -7580,7 +7533,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="6" t="s">
-        <v>797</v>
+        <v>784</v>
       </c>
       <c r="B216" s="28" t="s">
         <v>415</v>
@@ -7600,7 +7553,7 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
-        <v>798</v>
+        <v>785</v>
       </c>
       <c r="B217" s="28" t="s">
         <v>417</v>
@@ -7620,7 +7573,7 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
-        <v>799</v>
+        <v>786</v>
       </c>
       <c r="B218" s="28" t="s">
         <v>419</v>
@@ -7640,7 +7593,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>800</v>
+        <v>787</v>
       </c>
       <c r="B219" s="29" t="s">
         <v>422</v>
@@ -7660,7 +7613,7 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
       </c>
       <c r="B220" s="29" t="s">
         <v>423</v>
@@ -7680,7 +7633,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
-        <v>802</v>
+        <v>789</v>
       </c>
       <c r="B221" s="29" t="s">
         <v>424</v>
@@ -7700,7 +7653,7 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
-        <v>803</v>
+        <v>790</v>
       </c>
       <c r="B222" s="29" t="s">
         <v>425</v>
@@ -7720,7 +7673,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
-        <v>804</v>
+        <v>791</v>
       </c>
       <c r="B223" s="29" t="s">
         <v>426</v>
@@ -7740,7 +7693,7 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
-        <v>805</v>
+        <v>792</v>
       </c>
       <c r="B224" s="29" t="s">
         <v>427</v>
@@ -7760,7 +7713,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
-        <v>806</v>
+        <v>793</v>
       </c>
       <c r="B225" s="29" t="s">
         <v>428</v>
@@ -7780,7 +7733,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
-        <v>807</v>
+        <v>794</v>
       </c>
       <c r="B226" s="30" t="s">
         <v>429</v>
@@ -7800,7 +7753,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
-        <v>808</v>
+        <v>795</v>
       </c>
       <c r="B227" s="29" t="s">
         <v>430</v>
@@ -7820,7 +7773,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
-        <v>809</v>
+        <v>796</v>
       </c>
       <c r="B228" s="29" t="s">
         <v>431</v>
@@ -7840,7 +7793,7 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
-        <v>810</v>
+        <v>797</v>
       </c>
       <c r="B229" s="29" t="s">
         <v>432</v>
@@ -7860,7 +7813,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="B230" s="29" t="s">
         <v>433</v>
@@ -7880,7 +7833,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="6" t="s">
-        <v>812</v>
+        <v>799</v>
       </c>
       <c r="B231" s="29" t="s">
         <v>434</v>
@@ -7900,7 +7853,7 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="B232" s="29" t="s">
         <v>435</v>
@@ -7920,10 +7873,10 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="6" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="B233" s="29" t="s">
-        <v>571</v>
+        <v>903</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>436</v>
@@ -7940,13 +7893,13 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="B234" s="29" t="s">
-        <v>575</v>
+        <v>902</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="D234" s="5" t="b">
         <v>1</v>
@@ -7960,13 +7913,13 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="B235" s="29" t="s">
-        <v>574</v>
+        <v>901</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="D235" s="5" t="b">
         <v>1</v>
@@ -7980,13 +7933,13 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
-        <v>817</v>
+        <v>804</v>
       </c>
       <c r="B236" s="29" t="s">
-        <v>573</v>
+        <v>900</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="D236" s="5" t="b">
         <v>1</v>
@@ -8000,10 +7953,10 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
-        <v>818</v>
+        <v>805</v>
       </c>
       <c r="B237" s="30" t="s">
-        <v>572</v>
+        <v>898</v>
       </c>
       <c r="C237" s="20" t="s">
         <v>437</v>
@@ -8020,7 +7973,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
-        <v>819</v>
+        <v>806</v>
       </c>
       <c r="B238" s="29" t="s">
         <v>438</v>
@@ -8040,7 +7993,7 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
-        <v>820</v>
+        <v>807</v>
       </c>
       <c r="B239" s="30" t="s">
         <v>440</v>
@@ -8060,7 +8013,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="B240" s="29" t="s">
         <v>442</v>
@@ -8080,7 +8033,7 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="6" t="s">
-        <v>822</v>
+        <v>809</v>
       </c>
       <c r="B241" s="29" t="s">
         <v>444</v>
@@ -8100,7 +8053,7 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
-        <v>823</v>
+        <v>810</v>
       </c>
       <c r="B242" s="29" t="s">
         <v>446</v>
@@ -8120,7 +8073,7 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="6" t="s">
-        <v>824</v>
+        <v>811</v>
       </c>
       <c r="B243" s="29" t="s">
         <v>448</v>
@@ -8140,7 +8093,7 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
-        <v>825</v>
+        <v>812</v>
       </c>
       <c r="B244" s="29" t="s">
         <v>450</v>
@@ -8160,7 +8113,7 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
-        <v>826</v>
+        <v>813</v>
       </c>
       <c r="B245" s="29" t="s">
         <v>452</v>
@@ -8180,7 +8133,7 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
-        <v>827</v>
+        <v>814</v>
       </c>
       <c r="B246" s="32" t="s">
         <v>454</v>
@@ -8200,13 +8153,13 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="6" t="s">
-        <v>828</v>
+        <v>815</v>
       </c>
       <c r="B247" s="29" t="s">
-        <v>570</v>
+        <v>899</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="D247" s="5" t="b">
         <v>1</v>
@@ -8220,10 +8173,10 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
-        <v>829</v>
+        <v>816</v>
       </c>
       <c r="B248" s="29" t="s">
-        <v>569</v>
+        <v>897</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>456</v>
@@ -8240,7 +8193,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="6" t="s">
-        <v>830</v>
+        <v>817</v>
       </c>
       <c r="B249" s="31" t="s">
         <v>463</v>
@@ -8260,7 +8213,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
-        <v>831</v>
+        <v>818</v>
       </c>
       <c r="B250" s="31" t="s">
         <v>465</v>
@@ -8280,7 +8233,7 @@
     </row>
     <row r="251" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="6" t="s">
-        <v>832</v>
+        <v>819</v>
       </c>
       <c r="B251" s="31" t="s">
         <v>467</v>
@@ -8300,7 +8253,7 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
-        <v>833</v>
+        <v>820</v>
       </c>
       <c r="B252" s="27" t="s">
         <v>468</v>
@@ -8320,7 +8273,7 @@
     </row>
     <row r="253" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" s="6" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
       <c r="B253" s="27" t="s">
         <v>470</v>
@@ -8340,13 +8293,13 @@
     </row>
     <row r="254" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A254" s="6" t="s">
-        <v>835</v>
+        <v>822</v>
       </c>
       <c r="B254" s="28" t="s">
-        <v>576</v>
+        <v>894</v>
       </c>
       <c r="C254" s="22" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D254" s="25" t="b">
         <v>1</v>
@@ -8360,19 +8313,19 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="6" t="s">
-        <v>836</v>
+        <v>823</v>
       </c>
       <c r="B255" s="28" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="C255" s="22" t="s">
-        <v>581</v>
+        <v>538</v>
       </c>
       <c r="D255" s="25" t="b">
         <v>1</v>
       </c>
       <c r="E255" s="18" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F255" s="18" t="s">
         <v>79</v>
@@ -8380,19 +8333,19 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
-        <v>837</v>
+        <v>824</v>
       </c>
       <c r="B256" s="28" t="s">
-        <v>566</v>
-      </c>
-      <c r="C256" s="22" t="s">
-        <v>539</v>
+        <v>561</v>
+      </c>
+      <c r="C256" s="23" t="s">
+        <v>540</v>
       </c>
       <c r="D256" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="E256" s="18" t="s">
-        <v>540</v>
+      <c r="E256" s="19" t="s">
+        <v>473</v>
       </c>
       <c r="F256" s="18" t="s">
         <v>79</v>
@@ -8400,19 +8353,19 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="6" t="s">
-        <v>838</v>
+        <v>825</v>
       </c>
       <c r="B257" s="28" t="s">
-        <v>565</v>
-      </c>
-      <c r="C257" s="23" t="s">
+        <v>896</v>
+      </c>
+      <c r="C257" s="22" t="s">
+        <v>569</v>
+      </c>
+      <c r="D257" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E257" s="18" t="s">
         <v>541</v>
-      </c>
-      <c r="D257" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E257" s="19" t="s">
-        <v>473</v>
       </c>
       <c r="F257" s="18" t="s">
         <v>79</v>
@@ -8420,19 +8373,19 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="6" t="s">
-        <v>839</v>
+        <v>826</v>
       </c>
       <c r="B258" s="28" t="s">
-        <v>564</v>
-      </c>
-      <c r="C258" s="22" t="s">
-        <v>582</v>
+        <v>560</v>
+      </c>
+      <c r="C258" s="24" t="s">
+        <v>542</v>
       </c>
       <c r="D258" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="E258" s="18" t="s">
-        <v>542</v>
+      <c r="E258" s="19" t="s">
+        <v>543</v>
       </c>
       <c r="F258" s="18" t="s">
         <v>79</v>
@@ -8440,19 +8393,19 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="6" t="s">
-        <v>840</v>
+        <v>827</v>
       </c>
       <c r="B259" s="28" t="s">
-        <v>563</v>
-      </c>
-      <c r="C259" s="24" t="s">
-        <v>543</v>
+        <v>559</v>
+      </c>
+      <c r="C259" s="22" t="s">
+        <v>544</v>
       </c>
       <c r="D259" s="25" t="b">
         <v>1</v>
       </c>
       <c r="E259" s="19" t="s">
-        <v>544</v>
+        <v>475</v>
       </c>
       <c r="F259" s="18" t="s">
         <v>79</v>
@@ -8460,10 +8413,10 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
-        <v>841</v>
+        <v>828</v>
       </c>
       <c r="B260" s="28" t="s">
-        <v>562</v>
+        <v>895</v>
       </c>
       <c r="C260" s="22" t="s">
         <v>545</v>
@@ -8471,8 +8424,8 @@
       <c r="D260" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="E260" s="19" t="s">
-        <v>475</v>
+      <c r="E260" s="18" t="s">
+        <v>546</v>
       </c>
       <c r="F260" s="18" t="s">
         <v>79</v>
@@ -8480,33 +8433,33 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="6" t="s">
-        <v>842</v>
+        <v>829</v>
       </c>
       <c r="B261" s="28" t="s">
-        <v>561</v>
-      </c>
-      <c r="C261" s="22" t="s">
-        <v>546</v>
-      </c>
-      <c r="D261" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E261" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="C261" s="21" t="s">
         <v>547</v>
       </c>
-      <c r="F261" s="18" t="s">
+      <c r="D261" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E261" s="21" t="s">
+        <v>478</v>
+      </c>
+      <c r="F261" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="6" t="s">
-        <v>843</v>
+        <v>830</v>
       </c>
       <c r="B262" s="28" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C262" s="21" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D262" s="3" t="b">
         <v>0</v>
@@ -8520,16 +8473,16 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
-        <v>844</v>
+        <v>831</v>
       </c>
       <c r="B263" s="28" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C263" s="21" t="s">
         <v>548</v>
       </c>
       <c r="D263" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E263" s="21" t="s">
         <v>478</v>
@@ -8540,10 +8493,10 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="6" t="s">
-        <v>845</v>
+        <v>832</v>
       </c>
       <c r="B264" s="28" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C264" s="21" t="s">
         <v>549</v>
@@ -8560,10 +8513,10 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="6" t="s">
-        <v>846</v>
+        <v>833</v>
       </c>
       <c r="B265" s="28" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C265" s="21" t="s">
         <v>550</v>
@@ -8580,13 +8533,13 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="6" t="s">
-        <v>847</v>
+        <v>834</v>
       </c>
       <c r="B266" s="28" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C266" s="21" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D266" s="3" t="b">
         <v>1</v>
@@ -8600,10 +8553,10 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="6" t="s">
-        <v>848</v>
+        <v>835</v>
       </c>
       <c r="B267" s="28" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C267" s="21" t="s">
         <v>551</v>
@@ -8620,16 +8573,16 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="6" t="s">
-        <v>849</v>
+        <v>836</v>
       </c>
       <c r="B268" s="28" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C268" s="21" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D268" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E268" s="21" t="s">
         <v>478</v>
@@ -8640,13 +8593,13 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
-        <v>850</v>
+        <v>837</v>
       </c>
       <c r="B269" s="28" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C269" s="21" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D269" s="3" t="b">
         <v>0</v>
@@ -8660,13 +8613,13 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
-        <v>851</v>
+        <v>838</v>
       </c>
       <c r="B270" s="28" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C270" s="21" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D270" s="3" t="b">
         <v>0</v>
@@ -8680,16 +8633,16 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="6" t="s">
-        <v>852</v>
+        <v>839</v>
       </c>
       <c r="B271" s="28" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C271" s="21" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="D271" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E271" s="21" t="s">
         <v>478</v>
@@ -8700,16 +8653,16 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
-        <v>853</v>
+        <v>840</v>
       </c>
       <c r="B272" s="28" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C272" s="21" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="D272" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E272" s="21" t="s">
         <v>478</v>
@@ -8720,13 +8673,13 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="6" t="s">
-        <v>854</v>
+        <v>841</v>
       </c>
       <c r="B273" s="28" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C273" s="21" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D273" s="3" t="b">
         <v>0</v>
@@ -8740,19 +8693,19 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
-        <v>855</v>
+        <v>842</v>
       </c>
       <c r="B274" s="28" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C274" s="21" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="D274" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E274" s="21" t="s">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="F274" s="21" t="s">
         <v>79</v>
@@ -8760,13 +8713,13 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="6" t="s">
-        <v>856</v>
+        <v>843</v>
       </c>
       <c r="B275" s="28" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C275" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D275" s="3" t="b">
         <v>0</v>
@@ -8780,16 +8733,16 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="6" t="s">
-        <v>857</v>
+        <v>844</v>
       </c>
       <c r="B276" s="28" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C276" s="21" t="s">
         <v>554</v>
       </c>
       <c r="D276" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E276" s="21" t="s">
         <v>492</v>
@@ -8800,16 +8753,16 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="6" t="s">
-        <v>858</v>
+        <v>845</v>
       </c>
       <c r="B277" s="28" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C277" s="21" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D277" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E277" s="21" t="s">
         <v>492</v>
@@ -8820,13 +8773,13 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
-        <v>859</v>
+        <v>846</v>
       </c>
       <c r="B278" s="28" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C278" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D278" s="3" t="b">
         <v>0</v>
@@ -8840,13 +8793,13 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="6" t="s">
-        <v>860</v>
+        <v>847</v>
       </c>
       <c r="B279" s="28" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C279" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D279" s="3" t="b">
         <v>0</v>
@@ -8860,16 +8813,16 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
-        <v>861</v>
+        <v>848</v>
       </c>
       <c r="B280" s="28" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C280" s="21" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D280" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E280" s="21" t="s">
         <v>492</v>
@@ -8880,16 +8833,16 @@
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
-        <v>862</v>
+        <v>849</v>
       </c>
       <c r="B281" s="28" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C281" s="21" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D281" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E281" s="21" t="s">
         <v>492</v>
@@ -8900,13 +8853,13 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
-        <v>863</v>
+        <v>850</v>
       </c>
       <c r="B282" s="28" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C282" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D282" s="3" t="b">
         <v>0</v>
@@ -8920,13 +8873,13 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
-        <v>864</v>
+        <v>851</v>
       </c>
       <c r="B283" s="28" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C283" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D283" s="3" t="b">
         <v>0</v>
@@ -8940,13 +8893,13 @@
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
-        <v>865</v>
+        <v>852</v>
       </c>
       <c r="B284" s="28" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C284" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D284" s="3" t="b">
         <v>0</v>
@@ -8960,13 +8913,13 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="6" t="s">
-        <v>866</v>
+        <v>853</v>
       </c>
       <c r="B285" s="28" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C285" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D285" s="3" t="b">
         <v>0</v>
@@ -8980,13 +8933,13 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="6" t="s">
-        <v>867</v>
+        <v>854</v>
       </c>
       <c r="B286" s="28" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C286" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D286" s="3" t="b">
         <v>0</v>
@@ -9000,13 +8953,13 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="6" t="s">
-        <v>868</v>
+        <v>855</v>
       </c>
       <c r="B287" s="28" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C287" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D287" s="3" t="b">
         <v>0</v>
@@ -9020,13 +8973,13 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="6" t="s">
-        <v>869</v>
+        <v>856</v>
       </c>
       <c r="B288" s="28" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C288" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D288" s="3" t="b">
         <v>0</v>
@@ -9040,13 +8993,13 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="6" t="s">
-        <v>870</v>
+        <v>857</v>
       </c>
       <c r="B289" s="28" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C289" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D289" s="3" t="b">
         <v>0</v>
@@ -9060,13 +9013,13 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
-        <v>871</v>
+        <v>858</v>
       </c>
       <c r="B290" s="28" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C290" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D290" s="3" t="b">
         <v>0</v>
@@ -9080,13 +9033,13 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="6" t="s">
-        <v>872</v>
+        <v>859</v>
       </c>
       <c r="B291" s="28" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C291" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D291" s="3" t="b">
         <v>0</v>
@@ -9100,13 +9053,13 @@
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
-        <v>873</v>
+        <v>860</v>
       </c>
       <c r="B292" s="28" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C292" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D292" s="3" t="b">
         <v>0</v>
@@ -9120,13 +9073,13 @@
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="6" t="s">
-        <v>874</v>
+        <v>861</v>
       </c>
       <c r="B293" s="28" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C293" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D293" s="3" t="b">
         <v>0</v>
@@ -9140,13 +9093,13 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
-        <v>875</v>
+        <v>862</v>
       </c>
       <c r="B294" s="28" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C294" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D294" s="3" t="b">
         <v>0</v>
@@ -9160,13 +9113,13 @@
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="6" t="s">
-        <v>876</v>
+        <v>863</v>
       </c>
       <c r="B295" s="28" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C295" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D295" s="3" t="b">
         <v>0</v>
@@ -9180,16 +9133,16 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="6" t="s">
-        <v>877</v>
+        <v>864</v>
       </c>
       <c r="B296" s="28" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C296" s="21" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="D296" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E296" s="21" t="s">
         <v>492</v>
@@ -9200,16 +9153,16 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="6" t="s">
-        <v>878</v>
+        <v>865</v>
       </c>
       <c r="B297" s="28" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C297" s="21" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D297" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E297" s="21" t="s">
         <v>492</v>
@@ -9220,13 +9173,13 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
-        <v>879</v>
+        <v>866</v>
       </c>
       <c r="B298" s="28" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C298" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D298" s="3" t="b">
         <v>0</v>
@@ -9240,13 +9193,13 @@
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="6" t="s">
-        <v>880</v>
+        <v>867</v>
       </c>
       <c r="B299" s="28" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C299" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D299" s="3" t="b">
         <v>0</v>
@@ -9260,13 +9213,13 @@
     </row>
     <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
-        <v>881</v>
+        <v>868</v>
       </c>
       <c r="B300" s="28" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C300" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D300" s="3" t="b">
         <v>0</v>
@@ -9280,13 +9233,13 @@
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
-        <v>882</v>
+        <v>869</v>
       </c>
       <c r="B301" s="28" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C301" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D301" s="3" t="b">
         <v>0</v>
@@ -9300,13 +9253,13 @@
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="6" t="s">
-        <v>883</v>
+        <v>870</v>
       </c>
       <c r="B302" s="28" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C302" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D302" s="3" t="b">
         <v>0</v>
@@ -9320,13 +9273,13 @@
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="6" t="s">
-        <v>884</v>
+        <v>871</v>
       </c>
       <c r="B303" s="28" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C303" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D303" s="3" t="b">
         <v>0</v>
@@ -9340,13 +9293,13 @@
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
-        <v>885</v>
+        <v>872</v>
       </c>
       <c r="B304" s="28" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C304" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D304" s="3" t="b">
         <v>0</v>
@@ -9360,13 +9313,13 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="6" t="s">
-        <v>886</v>
+        <v>873</v>
       </c>
       <c r="B305" s="28" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C305" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D305" s="3" t="b">
         <v>0</v>
@@ -9380,13 +9333,13 @@
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
-        <v>887</v>
+        <v>874</v>
       </c>
       <c r="B306" s="28" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C306" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D306" s="3" t="b">
         <v>0</v>
@@ -9400,13 +9353,13 @@
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
-        <v>888</v>
+        <v>875</v>
       </c>
       <c r="B307" s="28" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C307" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D307" s="3" t="b">
         <v>0</v>
@@ -9420,13 +9373,13 @@
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
-        <v>889</v>
+        <v>876</v>
       </c>
       <c r="B308" s="28" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C308" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D308" s="3" t="b">
         <v>0</v>
@@ -9440,13 +9393,13 @@
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="6" t="s">
-        <v>890</v>
+        <v>877</v>
       </c>
       <c r="B309" s="28" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C309" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D309" s="3" t="b">
         <v>0</v>
@@ -9460,13 +9413,13 @@
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="6" t="s">
-        <v>891</v>
+        <v>878</v>
       </c>
       <c r="B310" s="28" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C310" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D310" s="3" t="b">
         <v>0</v>
@@ -9480,13 +9433,13 @@
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
-        <v>892</v>
+        <v>879</v>
       </c>
       <c r="B311" s="28" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C311" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D311" s="3" t="b">
         <v>0</v>
@@ -9500,13 +9453,13 @@
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
-        <v>893</v>
+        <v>880</v>
       </c>
       <c r="B312" s="28" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C312" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D312" s="3" t="b">
         <v>0</v>
@@ -9520,13 +9473,13 @@
     </row>
     <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="6" t="s">
-        <v>894</v>
+        <v>881</v>
       </c>
       <c r="B313" s="28" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C313" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D313" s="3" t="b">
         <v>0</v>
@@ -9540,13 +9493,13 @@
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="6" t="s">
-        <v>895</v>
+        <v>882</v>
       </c>
       <c r="B314" s="28" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C314" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D314" s="3" t="b">
         <v>0</v>
@@ -9560,13 +9513,13 @@
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="6" t="s">
-        <v>896</v>
+        <v>883</v>
       </c>
       <c r="B315" s="28" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C315" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D315" s="3" t="b">
         <v>0</v>
@@ -9580,13 +9533,13 @@
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
-        <v>897</v>
+        <v>884</v>
       </c>
       <c r="B316" s="28" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C316" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D316" s="3" t="b">
         <v>0</v>
@@ -9600,13 +9553,13 @@
     </row>
     <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="6" t="s">
-        <v>898</v>
+        <v>885</v>
       </c>
       <c r="B317" s="28" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C317" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D317" s="3" t="b">
         <v>0</v>
@@ -9620,13 +9573,13 @@
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="6" t="s">
-        <v>899</v>
+        <v>886</v>
       </c>
       <c r="B318" s="28" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C318" s="21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D318" s="3" t="b">
         <v>0</v>
@@ -9638,21 +9591,21 @@
         <v>79</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="6" t="s">
-        <v>900</v>
+        <v>887</v>
       </c>
       <c r="B319" s="28" t="s">
-        <v>536</v>
-      </c>
-      <c r="C319" s="21" t="s">
-        <v>554</v>
-      </c>
-      <c r="D319" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E319" s="21" t="s">
-        <v>492</v>
+        <v>563</v>
+      </c>
+      <c r="C319" s="22" t="s">
+        <v>892</v>
+      </c>
+      <c r="D319" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E319" s="19" t="s">
+        <v>891</v>
       </c>
       <c r="F319" s="21" t="s">
         <v>79</v>
@@ -9660,37 +9613,36 @@
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="6" t="s">
-        <v>901</v>
+        <v>888</v>
       </c>
       <c r="B320" s="28" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C320" s="6" t="s">
-        <v>560</v>
+        <v>893</v>
       </c>
       <c r="D320" s="9" t="b">
         <v>1</v>
       </c>
       <c r="E320" s="6" t="s">
-        <v>558</v>
-      </c>
-      <c r="F320" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="F320" s="21" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F320"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text=".txt">
-      <formula>NOT(ISERROR(SEARCH(".txt",B1)))</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="[">
       <formula>NOT(ISERROR(SEARCH("[",B1)))</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text=".txt">
+      <formula>NOT(ISERROR(SEARCH(".txt",B1)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Still tweaking TOMES patterns.
</commit_message>
<xml_diff>
--- a/dictionaries/TOMES_Entity_Dictionary.xlsx
+++ b/dictionaries/TOMES_Entity_Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4050" windowWidth="20400" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="20400" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -2733,13 +2733,13 @@
     <t>TOMES_PATTERN: {"(?i)House(?-i) (?i)Bill(?-i)", "H", "HB", "H. B.", "H.B."}, {"" , " "}, {"[0-9]{1,4}"}</t>
   </si>
   <si>
-    <t>TOMES_PATTERN: {"(?i)General(?-i) (?i)Statute(?-i)", "GS", "G. S.", "G.S."}, {" "}, {"", "§", "§ "}, {"[12][0-9]{0,2}[a-zA-Z]{0,1}"}</t>
-  </si>
-  <si>
     <t>TOMES_PATTERN: {"(?i)Executive(?-i) (?i)Order(?-i)", "(?i)Executive(?-i) (?i)Order(?-i) (?i)No(?-i).", "EO", "E. O."}, {" "}, {"[0-9]{1,3}"}</t>
   </si>
   <si>
     <t>TOMES_PATTERN: {"([1-9]|[1-5][0-9])"}, {" "}, {"(CFR|C\.F\.R)"}, {"", " §"}, {" "}, {"[0-9]{1,4}(\.[1-9]{1,4}){0,1}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"(?i)General(?-i) (?i)Statute(?-i)", "GS", "G. S.", "G.S."}, {"", " "}, {"", "§", "§ "}, {"[12][0-9]{0,2}[a-zA-Z]{0,1}"}</t>
   </si>
 </sst>
 </file>
@@ -3217,8 +3217,8 @@
   <dimension ref="A1:F320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B235" sqref="B235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7876,7 +7876,7 @@
         <v>801</v>
       </c>
       <c r="B233" s="29" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>436</v>
@@ -7896,7 +7896,7 @@
         <v>802</v>
       </c>
       <c r="B234" s="29" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>568</v>
@@ -7916,7 +7916,7 @@
         <v>803</v>
       </c>
       <c r="B235" s="29" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>567</v>

</xml_diff>

<commit_message>
Tweaked soem patterns and documentation.
</commit_message>
<xml_diff>
--- a/dictionaries/TOMES_Entity_Dictionary.xlsx
+++ b/dictionaries/TOMES_Entity_Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4500" windowWidth="20400" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4950" windowWidth="20400" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -2706,24 +2706,15 @@
     <t>TOMES.email_address</t>
   </si>
   <si>
-    <t>An electronic mailing address. Note, in North Carolina email addresses fall under the legal definition of PII in G.S. 14-113.20, G.S. 132 exempts them from the confidentiality requirements.</t>
-  </si>
-  <si>
     <t>A Uniform Resource Locator (URL) or File Transfer Protocal (FTP) string reference.</t>
   </si>
   <si>
     <t>TOMES_PATTERN: {"((0[0-9])|(1[0-2])|(2[1-9])|(3[0-2])|(6[1-9])|(7[0-2])|80)[0-9]{2}-{0,1}[0-9]{4}-{0,1}[0-9]"}, {" ", "-"}, {"[0-9]{6,17}"}</t>
   </si>
   <si>
-    <t>TOMES_PATTERN: {"(?!000)"}, {"([0-6][0-9]{2}|7([0-6][0-9]{1}|7[012]))"}, {" ", "-"}, {"(?!00)"}, {"[0-9]{2}"}, {" ", "-"}, {"(?!0000)"}, {"[0-9]{4}"}</t>
-  </si>
-  <si>
     <t>TOMES_PATTERN: {"[0-9]{4}"}, {" ", "-"}, {"[0-9]{4}"}, {" ", "-"}, {"[0-9]{4}"}, {"", " ", "-"}, {"[0-9]{4}"}</t>
   </si>
   <si>
-    <t>TOMES_PATTERN: {"([1-9]|[1-5][0-9])"}, {" "}, {"(USC|U\.S\.C)"}, {"", " "}, {"(§{1,2}){0,1}"}, {" "}, {"[1-9][0-9]{0,2}(-[1-9][0-9]{0,3}){0,1}"}</t>
-  </si>
-  <si>
     <t>TOMES_PATTERN: {"([1-9]|[1-3][0-9])[A-Z]{0,1}"}, {" "}, {"N.C. Admin Code", "NC Admin Code", "NCAC"}, {" "}, {"[1-9][0-9]{0,1}[A-Z]\.[0-9]{1,4}"}</t>
   </si>
   <si>
@@ -2740,6 +2731,15 @@
   </si>
   <si>
     <t>TOMES_PATTERN: {"(?i)General(?-i) (?i)Statute(?-i)", "GS", "G. S.", "G.S."}, {"", " "}, {"", "§", "§ "}, {"[12][0-9]{0,2}[a-zA-Z]{0,1}"}</t>
+  </si>
+  <si>
+    <t>An electronic mailing address. In North Carolina email addresses fall under the legal definition of PII in G.S. 14-113.20, but G.S. 132 exempts them from confidentiality requirements.</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"(?!000)"}, {"([0-6][0-9]{2}|7([0-6][0-9]{1}|7[012]))"}, {"", " ", "-"}, {"(?!00)"}, {"[0-9]{2}"}, {" ", "-"}, {"(?!0000)"}, {"[0-9]{4}"}</t>
+  </si>
+  <si>
+    <t>TOMES_PATTERN: {"([1-9]|[1-5][0-9])"}, {" "}, {"(USC|U\.S\.C)"}, {"", " (§{1,2}){0,1}"}, {" "}, {"[1-9][0-9]{0,2}(-[1-9][0-9]{0,3}){0,1}"}</t>
   </si>
 </sst>
 </file>
@@ -3214,11 +3214,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B235" sqref="B235"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B248" sqref="B248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3251,7 +3252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>570</v>
       </c>
@@ -3271,7 +3272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>571</v>
       </c>
@@ -3291,7 +3292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>572</v>
       </c>
@@ -3311,7 +3312,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>573</v>
       </c>
@@ -3331,7 +3332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>574</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>575</v>
       </c>
@@ -3371,7 +3372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>576</v>
       </c>
@@ -3391,7 +3392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>577</v>
       </c>
@@ -3411,7 +3412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>578</v>
       </c>
@@ -3431,7 +3432,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>579</v>
       </c>
@@ -3451,7 +3452,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>580</v>
       </c>
@@ -3471,7 +3472,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>581</v>
       </c>
@@ -3491,7 +3492,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>582</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>583</v>
       </c>
@@ -3531,7 +3532,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>584</v>
       </c>
@@ -3551,7 +3552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>585</v>
       </c>
@@ -3571,7 +3572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>586</v>
       </c>
@@ -3591,7 +3592,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>587</v>
       </c>
@@ -3611,7 +3612,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>588</v>
       </c>
@@ -3631,7 +3632,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>589</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>590</v>
       </c>
@@ -3671,7 +3672,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>591</v>
       </c>
@@ -3691,7 +3692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>592</v>
       </c>
@@ -3711,7 +3712,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>593</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>594</v>
       </c>
@@ -3751,7 +3752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>595</v>
       </c>
@@ -3771,7 +3772,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>596</v>
       </c>
@@ -3791,7 +3792,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>597</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>598</v>
       </c>
@@ -3831,7 +3832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>599</v>
       </c>
@@ -3851,7 +3852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>600</v>
       </c>
@@ -3871,7 +3872,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>601</v>
       </c>
@@ -3891,7 +3892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>602</v>
       </c>
@@ -3911,7 +3912,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>603</v>
       </c>
@@ -3931,7 +3932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>604</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>605</v>
       </c>
@@ -3971,7 +3972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="56.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>606</v>
       </c>
@@ -3991,7 +3992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>607</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>608</v>
       </c>
@@ -4031,7 +4032,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>609</v>
       </c>
@@ -4051,7 +4052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>610</v>
       </c>
@@ -4071,7 +4072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>611</v>
       </c>
@@ -4091,7 +4092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>612</v>
       </c>
@@ -4111,7 +4112,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>613</v>
       </c>
@@ -4131,7 +4132,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>614</v>
       </c>
@@ -4151,7 +4152,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>615</v>
       </c>
@@ -4171,7 +4172,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>616</v>
       </c>
@@ -4191,7 +4192,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>617</v>
       </c>
@@ -4211,7 +4212,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>618</v>
       </c>
@@ -4231,7 +4232,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>619</v>
       </c>
@@ -4251,7 +4252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>620</v>
       </c>
@@ -4271,7 +4272,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>621</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>622</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>623</v>
       </c>
@@ -4331,7 +4332,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>624</v>
       </c>
@@ -4351,7 +4352,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>625</v>
       </c>
@@ -4371,7 +4372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>626</v>
       </c>
@@ -4391,7 +4392,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>627</v>
       </c>
@@ -4411,7 +4412,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>628</v>
       </c>
@@ -4431,7 +4432,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>629</v>
       </c>
@@ -4451,7 +4452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>630</v>
       </c>
@@ -4471,7 +4472,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>631</v>
       </c>
@@ -4491,7 +4492,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>632</v>
       </c>
@@ -4511,7 +4512,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>633</v>
       </c>
@@ -4531,7 +4532,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>634</v>
       </c>
@@ -4551,7 +4552,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>635</v>
       </c>
@@ -4571,7 +4572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>636</v>
       </c>
@@ -4591,7 +4592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>637</v>
       </c>
@@ -4611,7 +4612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>638</v>
       </c>
@@ -4631,7 +4632,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>639</v>
       </c>
@@ -4651,7 +4652,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>640</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>641</v>
       </c>
@@ -4691,7 +4692,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>642</v>
       </c>
@@ -4711,7 +4712,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>643</v>
       </c>
@@ -4731,7 +4732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>644</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>645</v>
       </c>
@@ -4771,7 +4772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>646</v>
       </c>
@@ -4791,7 +4792,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>647</v>
       </c>
@@ -4811,7 +4812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>648</v>
       </c>
@@ -4831,7 +4832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>649</v>
       </c>
@@ -4851,7 +4852,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>650</v>
       </c>
@@ -4871,7 +4872,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>651</v>
       </c>
@@ -4891,7 +4892,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>652</v>
       </c>
@@ -4911,7 +4912,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>653</v>
       </c>
@@ -4931,7 +4932,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>654</v>
       </c>
@@ -4951,7 +4952,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>655</v>
       </c>
@@ -4971,7 +4972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>656</v>
       </c>
@@ -4991,7 +4992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>657</v>
       </c>
@@ -5011,7 +5012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>658</v>
       </c>
@@ -5031,7 +5032,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>659</v>
       </c>
@@ -5051,7 +5052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>660</v>
       </c>
@@ -5071,7 +5072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>661</v>
       </c>
@@ -5091,7 +5092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>662</v>
       </c>
@@ -5111,7 +5112,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>663</v>
       </c>
@@ -5131,7 +5132,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>664</v>
       </c>
@@ -5151,7 +5152,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>665</v>
       </c>
@@ -5171,7 +5172,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>666</v>
       </c>
@@ -5191,7 +5192,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>667</v>
       </c>
@@ -5211,7 +5212,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>668</v>
       </c>
@@ -5231,7 +5232,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>669</v>
       </c>
@@ -5251,7 +5252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>670</v>
       </c>
@@ -5271,7 +5272,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>671</v>
       </c>
@@ -5291,7 +5292,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>672</v>
       </c>
@@ -5311,7 +5312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>673</v>
       </c>
@@ -5331,7 +5332,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>674</v>
       </c>
@@ -5351,7 +5352,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>675</v>
       </c>
@@ -5371,7 +5372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>676</v>
       </c>
@@ -5391,7 +5392,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>677</v>
       </c>
@@ -5411,7 +5412,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>678</v>
       </c>
@@ -5431,7 +5432,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>679</v>
       </c>
@@ -5451,7 +5452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>680</v>
       </c>
@@ -5471,7 +5472,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>681</v>
       </c>
@@ -5491,7 +5492,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>682</v>
       </c>
@@ -5511,7 +5512,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>683</v>
       </c>
@@ -5531,7 +5532,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>684</v>
       </c>
@@ -5551,7 +5552,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>685</v>
       </c>
@@ -5571,7 +5572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>686</v>
       </c>
@@ -5591,7 +5592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>687</v>
       </c>
@@ -5611,7 +5612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>688</v>
       </c>
@@ -5631,7 +5632,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>689</v>
       </c>
@@ -5651,7 +5652,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>690</v>
       </c>
@@ -5671,7 +5672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>691</v>
       </c>
@@ -5691,7 +5692,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>692</v>
       </c>
@@ -5711,7 +5712,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>693</v>
       </c>
@@ -5731,7 +5732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>694</v>
       </c>
@@ -5751,7 +5752,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>695</v>
       </c>
@@ -5771,7 +5772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>696</v>
       </c>
@@ -5791,7 +5792,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>697</v>
       </c>
@@ -5811,7 +5812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>698</v>
       </c>
@@ -5831,7 +5832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>699</v>
       </c>
@@ -5851,7 +5852,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>700</v>
       </c>
@@ -5871,7 +5872,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>701</v>
       </c>
@@ -5891,7 +5892,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>702</v>
       </c>
@@ -5911,7 +5912,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>703</v>
       </c>
@@ -5931,7 +5932,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>704</v>
       </c>
@@ -5951,7 +5952,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>705</v>
       </c>
@@ -5971,7 +5972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>706</v>
       </c>
@@ -5991,7 +5992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>707</v>
       </c>
@@ -6011,7 +6012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>708</v>
       </c>
@@ -6031,7 +6032,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>709</v>
       </c>
@@ -6051,7 +6052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>710</v>
       </c>
@@ -6071,7 +6072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>711</v>
       </c>
@@ -6091,7 +6092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>712</v>
       </c>
@@ -6111,7 +6112,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>713</v>
       </c>
@@ -6131,7 +6132,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>714</v>
       </c>
@@ -6151,7 +6152,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>715</v>
       </c>
@@ -6171,7 +6172,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>716</v>
       </c>
@@ -6191,7 +6192,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>717</v>
       </c>
@@ -6211,7 +6212,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>718</v>
       </c>
@@ -6231,7 +6232,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>719</v>
       </c>
@@ -6251,7 +6252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>720</v>
       </c>
@@ -6271,7 +6272,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>721</v>
       </c>
@@ -6291,7 +6292,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>722</v>
       </c>
@@ -6311,7 +6312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>723</v>
       </c>
@@ -6331,7 +6332,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>724</v>
       </c>
@@ -6351,7 +6352,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>725</v>
       </c>
@@ -6371,7 +6372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>726</v>
       </c>
@@ -6391,7 +6392,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>727</v>
       </c>
@@ -6411,7 +6412,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
         <v>728</v>
       </c>
@@ -6431,7 +6432,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
         <v>729</v>
       </c>
@@ -6451,7 +6452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
         <v>730</v>
       </c>
@@ -6471,7 +6472,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
         <v>731</v>
       </c>
@@ -6491,7 +6492,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
         <v>732</v>
       </c>
@@ -6511,7 +6512,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
         <v>733</v>
       </c>
@@ -6531,7 +6532,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
         <v>734</v>
       </c>
@@ -6551,7 +6552,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
         <v>735</v>
       </c>
@@ -6571,7 +6572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
         <v>736</v>
       </c>
@@ -6591,7 +6592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
         <v>737</v>
       </c>
@@ -6611,7 +6612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
         <v>738</v>
       </c>
@@ -6631,7 +6632,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>739</v>
       </c>
@@ -6651,7 +6652,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
         <v>740</v>
       </c>
@@ -6671,7 +6672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
         <v>741</v>
       </c>
@@ -6691,7 +6692,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
         <v>742</v>
       </c>
@@ -6711,7 +6712,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
         <v>743</v>
       </c>
@@ -6731,7 +6732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>744</v>
       </c>
@@ -6751,7 +6752,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
         <v>745</v>
       </c>
@@ -6771,7 +6772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
         <v>746</v>
       </c>
@@ -6791,7 +6792,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>747</v>
       </c>
@@ -6811,7 +6812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
         <v>748</v>
       </c>
@@ -6831,7 +6832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
         <v>749</v>
       </c>
@@ -6851,7 +6852,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
         <v>750</v>
       </c>
@@ -6871,7 +6872,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
         <v>751</v>
       </c>
@@ -6891,7 +6892,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
         <v>752</v>
       </c>
@@ -6911,7 +6912,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
         <v>753</v>
       </c>
@@ -6931,7 +6932,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
         <v>754</v>
       </c>
@@ -6951,7 +6952,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="6" t="s">
         <v>755</v>
       </c>
@@ -6971,7 +6972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
         <v>756</v>
       </c>
@@ -6991,7 +6992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="6" t="s">
         <v>757</v>
       </c>
@@ -7011,7 +7012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
         <v>758</v>
       </c>
@@ -7031,7 +7032,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
         <v>759</v>
       </c>
@@ -7051,7 +7052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
         <v>760</v>
       </c>
@@ -7071,7 +7072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
         <v>761</v>
       </c>
@@ -7091,7 +7092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
         <v>762</v>
       </c>
@@ -7111,7 +7112,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
         <v>763</v>
       </c>
@@ -7131,7 +7132,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
         <v>764</v>
       </c>
@@ -7151,7 +7152,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
         <v>765</v>
       </c>
@@ -7171,7 +7172,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="6" t="s">
         <v>766</v>
       </c>
@@ -7191,7 +7192,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
         <v>767</v>
       </c>
@@ -7211,7 +7212,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="6" t="s">
         <v>768</v>
       </c>
@@ -7231,7 +7232,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="6" t="s">
         <v>769</v>
       </c>
@@ -7251,7 +7252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
         <v>770</v>
       </c>
@@ -7271,7 +7272,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="6" t="s">
         <v>771</v>
       </c>
@@ -7291,7 +7292,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
         <v>772</v>
       </c>
@@ -7311,7 +7312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
         <v>773</v>
       </c>
@@ -7331,7 +7332,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
         <v>774</v>
       </c>
@@ -7351,7 +7352,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="6" t="s">
         <v>775</v>
       </c>
@@ -7371,7 +7372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
         <v>776</v>
       </c>
@@ -7391,7 +7392,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="6" t="s">
         <v>777</v>
       </c>
@@ -7411,7 +7412,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
         <v>778</v>
       </c>
@@ -7431,7 +7432,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="6" t="s">
         <v>779</v>
       </c>
@@ -7451,7 +7452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
         <v>780</v>
       </c>
@@ -7471,7 +7472,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
         <v>781</v>
       </c>
@@ -7491,7 +7492,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
         <v>782</v>
       </c>
@@ -7511,7 +7512,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="6" t="s">
         <v>783</v>
       </c>
@@ -7531,7 +7532,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="6" t="s">
         <v>784</v>
       </c>
@@ -7551,7 +7552,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
         <v>785</v>
       </c>
@@ -7571,7 +7572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
         <v>786</v>
       </c>
@@ -7591,7 +7592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
         <v>787</v>
       </c>
@@ -7611,7 +7612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
         <v>788</v>
       </c>
@@ -7631,7 +7632,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="6" t="s">
         <v>789</v>
       </c>
@@ -7651,7 +7652,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
         <v>790</v>
       </c>
@@ -7671,7 +7672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="6" t="s">
         <v>791</v>
       </c>
@@ -7691,7 +7692,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
         <v>792</v>
       </c>
@@ -7711,7 +7712,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="6" t="s">
         <v>793</v>
       </c>
@@ -7731,7 +7732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
         <v>794</v>
       </c>
@@ -7751,7 +7752,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
         <v>795</v>
       </c>
@@ -7771,7 +7772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
         <v>796</v>
       </c>
@@ -7791,7 +7792,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
         <v>797</v>
       </c>
@@ -7811,7 +7812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
         <v>798</v>
       </c>
@@ -7831,7 +7832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="6" t="s">
         <v>799</v>
       </c>
@@ -7851,7 +7852,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
         <v>800</v>
       </c>
@@ -7876,7 +7877,7 @@
         <v>801</v>
       </c>
       <c r="B233" s="29" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>436</v>
@@ -7896,7 +7897,7 @@
         <v>802</v>
       </c>
       <c r="B234" s="29" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>568</v>
@@ -7916,7 +7917,7 @@
         <v>803</v>
       </c>
       <c r="B235" s="29" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>567</v>
@@ -7936,7 +7937,7 @@
         <v>804</v>
       </c>
       <c r="B236" s="29" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="C236" s="4" t="s">
         <v>566</v>
@@ -7956,7 +7957,7 @@
         <v>805</v>
       </c>
       <c r="B237" s="30" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="C237" s="20" t="s">
         <v>437</v>
@@ -7971,7 +7972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
         <v>806</v>
       </c>
@@ -7991,7 +7992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
         <v>807</v>
       </c>
@@ -8011,7 +8012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
         <v>808</v>
       </c>
@@ -8031,7 +8032,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="6" t="s">
         <v>809</v>
       </c>
@@ -8051,7 +8052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
         <v>810</v>
       </c>
@@ -8071,7 +8072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="6" t="s">
         <v>811</v>
       </c>
@@ -8091,7 +8092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
         <v>812</v>
       </c>
@@ -8111,7 +8112,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="6" t="s">
         <v>813</v>
       </c>
@@ -8131,7 +8132,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
         <v>814</v>
       </c>
@@ -8156,7 +8157,7 @@
         <v>815</v>
       </c>
       <c r="B247" s="29" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>565</v>
@@ -8176,7 +8177,7 @@
         <v>816</v>
       </c>
       <c r="B248" s="29" t="s">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>456</v>
@@ -8191,7 +8192,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="6" t="s">
         <v>817</v>
       </c>
@@ -8211,7 +8212,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
         <v>818</v>
       </c>
@@ -8231,7 +8232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="6" t="s">
         <v>819</v>
       </c>
@@ -8251,7 +8252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
         <v>820</v>
       </c>
@@ -8271,7 +8272,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="6" t="s">
         <v>821</v>
       </c>
@@ -8296,7 +8297,7 @@
         <v>822</v>
       </c>
       <c r="B254" s="28" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C254" s="22" t="s">
         <v>564</v>
@@ -8311,7 +8312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="6" t="s">
         <v>823</v>
       </c>
@@ -8331,7 +8332,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
         <v>824</v>
       </c>
@@ -8356,7 +8357,7 @@
         <v>825</v>
       </c>
       <c r="B257" s="28" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C257" s="22" t="s">
         <v>569</v>
@@ -8371,7 +8372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="6" t="s">
         <v>826</v>
       </c>
@@ -8391,7 +8392,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="6" t="s">
         <v>827</v>
       </c>
@@ -8416,7 +8417,7 @@
         <v>828</v>
       </c>
       <c r="B260" s="28" t="s">
-        <v>895</v>
+        <v>902</v>
       </c>
       <c r="C260" s="22" t="s">
         <v>545</v>
@@ -8431,7 +8432,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="6" t="s">
         <v>829</v>
       </c>
@@ -8451,7 +8452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="6" t="s">
         <v>830</v>
       </c>
@@ -8471,7 +8472,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
         <v>831</v>
       </c>
@@ -8491,7 +8492,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="6" t="s">
         <v>832</v>
       </c>
@@ -8511,7 +8512,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="6" t="s">
         <v>833</v>
       </c>
@@ -8531,7 +8532,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="6" t="s">
         <v>834</v>
       </c>
@@ -8551,7 +8552,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="6" t="s">
         <v>835</v>
       </c>
@@ -8571,7 +8572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="6" t="s">
         <v>836</v>
       </c>
@@ -8591,7 +8592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
         <v>837</v>
       </c>
@@ -8611,7 +8612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
         <v>838</v>
       </c>
@@ -8631,7 +8632,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="6" t="s">
         <v>839</v>
       </c>
@@ -8651,7 +8652,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
         <v>840</v>
       </c>
@@ -8671,7 +8672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="6" t="s">
         <v>841</v>
       </c>
@@ -8691,7 +8692,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
         <v>842</v>
       </c>
@@ -8711,7 +8712,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="6" t="s">
         <v>843</v>
       </c>
@@ -8731,7 +8732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="6" t="s">
         <v>844</v>
       </c>
@@ -8751,7 +8752,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="6" t="s">
         <v>845</v>
       </c>
@@ -8771,7 +8772,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
         <v>846</v>
       </c>
@@ -8791,7 +8792,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="6" t="s">
         <v>847</v>
       </c>
@@ -8811,7 +8812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
         <v>848</v>
       </c>
@@ -8831,7 +8832,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
         <v>849</v>
       </c>
@@ -8851,7 +8852,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
         <v>850</v>
       </c>
@@ -8871,7 +8872,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
         <v>851</v>
       </c>
@@ -8891,7 +8892,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
         <v>852</v>
       </c>
@@ -8911,7 +8912,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="6" t="s">
         <v>853</v>
       </c>
@@ -8931,7 +8932,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="6" t="s">
         <v>854</v>
       </c>
@@ -8951,7 +8952,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="6" t="s">
         <v>855</v>
       </c>
@@ -8971,7 +8972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="6" t="s">
         <v>856</v>
       </c>
@@ -8991,7 +8992,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="6" t="s">
         <v>857</v>
       </c>
@@ -9011,7 +9012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
         <v>858</v>
       </c>
@@ -9031,7 +9032,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="6" t="s">
         <v>859</v>
       </c>
@@ -9051,7 +9052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
         <v>860</v>
       </c>
@@ -9071,7 +9072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="6" t="s">
         <v>861</v>
       </c>
@@ -9091,7 +9092,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
         <v>862</v>
       </c>
@@ -9111,7 +9112,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="6" t="s">
         <v>863</v>
       </c>
@@ -9131,7 +9132,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="6" t="s">
         <v>864</v>
       </c>
@@ -9151,7 +9152,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="6" t="s">
         <v>865</v>
       </c>
@@ -9171,7 +9172,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
         <v>866</v>
       </c>
@@ -9191,7 +9192,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="6" t="s">
         <v>867</v>
       </c>
@@ -9211,7 +9212,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
         <v>868</v>
       </c>
@@ -9231,7 +9232,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
         <v>869</v>
       </c>
@@ -9251,7 +9252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="6" t="s">
         <v>870</v>
       </c>
@@ -9271,7 +9272,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="6" t="s">
         <v>871</v>
       </c>
@@ -9291,7 +9292,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
         <v>872</v>
       </c>
@@ -9311,7 +9312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="6" t="s">
         <v>873</v>
       </c>
@@ -9331,7 +9332,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
         <v>874</v>
       </c>
@@ -9351,7 +9352,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
         <v>875</v>
       </c>
@@ -9371,7 +9372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
         <v>876</v>
       </c>
@@ -9391,7 +9392,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="6" t="s">
         <v>877</v>
       </c>
@@ -9411,7 +9412,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="6" t="s">
         <v>878</v>
       </c>
@@ -9431,7 +9432,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
         <v>879</v>
       </c>
@@ -9451,7 +9452,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
         <v>880</v>
       </c>
@@ -9471,7 +9472,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="6" t="s">
         <v>881</v>
       </c>
@@ -9491,7 +9492,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="6" t="s">
         <v>882</v>
       </c>
@@ -9511,7 +9512,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="6" t="s">
         <v>883</v>
       </c>
@@ -9531,7 +9532,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
         <v>884</v>
       </c>
@@ -9551,7 +9552,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="6" t="s">
         <v>885</v>
       </c>
@@ -9571,7 +9572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="6" t="s">
         <v>886</v>
       </c>
@@ -9591,7 +9592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="319" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="6" t="s">
         <v>887</v>
       </c>
@@ -9599,7 +9600,7 @@
         <v>563</v>
       </c>
       <c r="C319" s="22" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="D319" s="25" t="b">
         <v>1</v>
@@ -9611,7 +9612,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="6" t="s">
         <v>888</v>
       </c>
@@ -9619,7 +9620,7 @@
         <v>558</v>
       </c>
       <c r="C320" s="6" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D320" s="9" t="b">
         <v>1</v>
@@ -9632,7 +9633,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F320"/>
+  <autoFilter ref="A1:F320">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="TOMES_PATTERN: {&quot;((0[0-9])|(1[0-2])|(2[1-9])|(3[0-2])|(6[1-9])|(7[0-2])|80)[0-9]{2}-{0,1}[0-9]{4}-{0,1}[0-9]&quot;}, {&quot; &quot;, &quot;-&quot;}, {&quot;[0-9]{6,17}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;(?!000)&quot;}, {&quot;([0-6][0-9]{2}|7([0-6][0-9]{1}|7[012]))&quot;}, {&quot; &quot;, &quot;-&quot;}, {&quot;(?!00)&quot;}, {&quot;[0-9]{2}&quot;}, {&quot; &quot;, &quot;-&quot;}, {&quot;(?!0000)&quot;}, {&quot;[0-9]{4}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;(?i)Executive(?-i) (?i)Order(?-i)&quot;, &quot;(?i)Executive(?-i) (?i)Order(?-i) (?i)No(?-i).&quot;, &quot;EO&quot;, &quot;E. O.&quot;}, {&quot; &quot;}, {&quot;[0-9]{1,3}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;(?i)General(?-i) (?i)Statute(?-i)&quot;, &quot;GS&quot;, &quot;G. S.&quot;, &quot;G.S.&quot;}, {&quot;&quot;, &quot; &quot;}, {&quot;&quot;, &quot;§&quot;, &quot;§ &quot;}, {&quot;[12][0-9]{0,2}[a-zA-Z]{0,1}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;(?i)House(?-i) (?i)Bill(?-i)&quot;, &quot;H&quot;, &quot;HB&quot;, &quot;H. B.&quot;, &quot;H.B.&quot;}, {&quot;&quot; , &quot; &quot;}, {&quot;[0-9]{1,4}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;(?i)Senate(?-i) (?i)Bill(?-i)&quot;, &quot;S&quot;, &quot;SB&quot;, &quot;S.B.&quot;, &quot;S. B.&quot;}, {&quot;&quot;, &quot; &quot;}, {&quot;[0-9]{1,4}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;([1-9]|[1-3][0-9])[A-Z]{0,1}&quot;}, {&quot; &quot;}, {&quot;N.C. Admin Code&quot;, &quot;NC Admin Code&quot;, &quot;NCAC&quot;}, {&quot; &quot;}, {&quot;[1-9][0-9]{0,1}[A-Z]\.[0-9]{1,4}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;([1-9]|[1-5][0-9])&quot;}, {&quot; &quot;}, {&quot;(CFR|C\.F\.R)&quot;}, {&quot;&quot;, &quot; §&quot;}, {&quot; &quot;}, {&quot;[0-9]{1,4}(\.[1-9]{1,4}){0,1}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;([1-9]|[1-5][0-9])&quot;}, {&quot; &quot;}, {&quot;(USC|U\.S\.C)&quot;}, {&quot;&quot;, &quot; &quot;}, {&quot;(§{1,2}){0,1}&quot;}, {&quot; &quot;}, {&quot;[1-9][0-9]{0,2}(-[1-9][0-9]{0,3}){0,1}&quot;}"/>
+        <filter val="TOMES_PATTERN: {&quot;[0-9]{4}&quot;}, {&quot; &quot;, &quot;-&quot;}, {&quot;[0-9]{4}&quot;}, {&quot; &quot;, &quot;-&quot;}, {&quot;[0-9]{4}&quot;}, {&quot;&quot;, &quot; &quot;, &quot;-&quot;}, {&quot;[0-9]{4}&quot;}"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="[">

</xml_diff>

<commit_message>
Updated docstrings and comments after proofreading.
</commit_message>
<xml_diff>
--- a/dictionaries/TOMES_Entity_Dictionary.xlsx
+++ b/dictionaries/TOMES_Entity_Dictionary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitin\Dropbox\TOMES\GitHub\tomes_entities\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{44026FF8-93C0-4F82-9689-13DEBCF61BB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8550" windowWidth="20400" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="9450" windowWidth="20400" windowHeight="10410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -1461,9 +1462,6 @@
     <t>TOMES_PATTERN: {"([1-9]|[1-3][0-9])[A-Z]{0,1}"}, {" "}, {"N.C. Admin", "NC Admin", "NCAC [1-9][0-9]{0,1}[A-Z] \.[0-9]{1,4}"}</t>
   </si>
   <si>
-    <t>To learn more about the rationale for the regular expression and TOMES Patterns, see the text files in the "./regexs" folder.</t>
-  </si>
-  <si>
     <t>A reference to a correctional institution.</t>
   </si>
   <si>
@@ -1472,12 +1470,15 @@
   </si>
   <si>
     <t>TOMES_PATTERN: {"(?!000)([0-6][0-9]{2}|7([0-6][0-9]{1}|7[012]))"}, {" ", "-"}, {"(?!00)[0-9]{2}"}, {" ", "-"}, {"(?!0000)[0-9]{4}"}</t>
+  </si>
+  <si>
+    <t>To learn more about the regular expression and TOMES Patterns, see the text files in the "./regexs" folder.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1927,11 +1928,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,7 +1949,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -1957,12 +1958,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B246" sqref="B246"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7083,10 +7084,10 @@
         <v>0243</v>
       </c>
       <c r="B244" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C244" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D244" s="8" t="b">
         <v>1</v>
@@ -7125,7 +7126,7 @@
         <v>0245</v>
       </c>
       <c r="B246" s="27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C246" s="21" t="s">
         <v>436</v>

</xml_diff>